<commit_message>
blackout stability fixed. PV sign fixed.
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\FC Microgrid\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DE2B72-2662-4368-91BB-9E226CB27C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BA3D5D-98FE-4051-BD5C-7A8BD6F8AC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
   <sheets>
     <sheet name="WTGmode" sheetId="13" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B20"/>
+      <selection activeCell="B4" sqref="B4:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -19989,7 +19989,7 @@
       </c>
       <c r="B2">
         <f ca="1">575+0.5*RAND()</f>
-        <v>575.43023478878047</v>
+        <v>575.07947980138613</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -19998,7 +19998,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B52" ca="1" si="0">575+0.5*RAND()</f>
-        <v>575.27133299908155</v>
+        <v>575.0990236261639</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20007,7 +20007,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>575.10270409131158</v>
+        <v>575.14098195430654</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -20016,7 +20016,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>575.11946824997915</v>
+        <v>575.46948768782011</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20025,7 +20025,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>575.21198970605269</v>
+        <v>575.28959086369991</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -20034,7 +20034,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>575.33242315611324</v>
+        <v>575.08508739193519</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -20043,7 +20043,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>575.31324030344399</v>
+        <v>575.40921028566561</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -20052,7 +20052,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>575.43828348139493</v>
+        <v>575.22689235635187</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -20061,7 +20061,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>575.1286783285542</v>
+        <v>575.31236283415558</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -20070,7 +20070,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>575.25167386696251</v>
+        <v>575.18250676537014</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -20079,7 +20079,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>575.3525279230272</v>
+        <v>575.41130810272409</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -20088,7 +20088,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>575.4676260443938</v>
+        <v>575.18697431565647</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -20097,7 +20097,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>575.0131378976364</v>
+        <v>575.05307307466194</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -20106,7 +20106,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>575.12013863735626</v>
+        <v>575.35778045770735</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -20115,7 +20115,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>575.20507877971011</v>
+        <v>575.23185861291381</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -20124,7 +20124,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>575.4843010027007</v>
+        <v>575.11731102905867</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -20133,7 +20133,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>575.14719133121275</v>
+        <v>575.09905003538756</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -20142,7 +20142,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>575.22398159056127</v>
+        <v>575.28315352592494</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -20151,7 +20151,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>575.35134764850648</v>
+        <v>575.12919225488008</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -20160,7 +20160,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>575.07298694809231</v>
+        <v>575.02259957096885</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -20169,7 +20169,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>575.06131984694321</v>
+        <v>575.43393524493649</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -20178,7 +20178,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>575.28553288770593</v>
+        <v>575.09471214091593</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -20187,7 +20187,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>575.33099288458948</v>
+        <v>575.38573388404859</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -20196,7 +20196,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>575.49506391647355</v>
+        <v>575.36832769833552</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -20205,7 +20205,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>575.3371727081809</v>
+        <v>575.41326872018749</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -20214,7 +20214,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>575.00109564446666</v>
+        <v>575.30777440185409</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -20223,7 +20223,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>575.46515428904081</v>
+        <v>575.38109108892922</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -20232,7 +20232,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>575.24039764480779</v>
+        <v>575.48303681589675</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -20241,7 +20241,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>575.38371186450399</v>
+        <v>575.30052355909777</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -20250,7 +20250,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>575.47182386608608</v>
+        <v>575.30648825082551</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -20259,7 +20259,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>575.49314329291678</v>
+        <v>575.03391164066841</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -20268,7 +20268,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>575.18136233845178</v>
+        <v>575.11048421156318</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -20277,7 +20277,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>575.41316147926273</v>
+        <v>575.2223110811351</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -20286,7 +20286,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>575.09397068167459</v>
+        <v>575.15980490267566</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -20295,7 +20295,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>575.17700693219626</v>
+        <v>575.42273095968733</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -20304,7 +20304,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>575.11595458135423</v>
+        <v>575.36882794896553</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -20313,7 +20313,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>575.49448066994603</v>
+        <v>575.31825798669138</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -20322,7 +20322,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>575.22558408556085</v>
+        <v>575.00387707081563</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -20331,7 +20331,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>575.13787534715891</v>
+        <v>575.36570150806881</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -20340,7 +20340,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>575.28493004029815</v>
+        <v>575.33895682141303</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -20349,7 +20349,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>575.23215861195285</v>
+        <v>575.12325847454861</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -20358,7 +20358,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>575.44711507198633</v>
+        <v>575.47389699066434</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -20367,7 +20367,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>575.18357493410838</v>
+        <v>575.11422650648944</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -20376,7 +20376,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>575.45948808000298</v>
+        <v>575.00754002671044</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -20385,7 +20385,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>575.054111749105</v>
+        <v>575.25102941803982</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -20394,7 +20394,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>575.44708103482014</v>
+        <v>575.47283372394725</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -20403,7 +20403,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>575.19999193798947</v>
+        <v>575.06946765544035</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -20412,7 +20412,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>575.48123562658725</v>
+        <v>575.27499655074837</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -20421,7 +20421,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>575.40011123568297</v>
+        <v>575.40372207320354</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -20430,7 +20430,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>575.26724441844704</v>
+        <v>575.17579901369129</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -20439,7 +20439,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>575.2144863008383</v>
+        <v>575.20998951612455</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -20448,7 +20448,7 @@
       </c>
       <c r="B53">
         <f ca="1">B52-RAND()</f>
-        <v>575.13578595608601</v>
+        <v>574.54820311023116</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -20457,7 +20457,7 @@
       </c>
       <c r="B54">
         <f t="shared" ref="B54:B113" ca="1" si="1">B53-RAND()</f>
-        <v>574.73799070931511</v>
+        <v>573.63267899932589</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -20466,7 +20466,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>574.66165733656146</v>
+        <v>572.72661322930901</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -20475,7 +20475,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>574.20845166749257</v>
+        <v>572.31407613919475</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -20484,7 +20484,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>573.50651988271034</v>
+        <v>571.36315831754564</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -20493,7 +20493,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>573.04241354670387</v>
+        <v>571.3525586030479</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -20502,7 +20502,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>572.11260924358305</v>
+        <v>570.42721571291918</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -20511,7 +20511,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>571.24881403076904</v>
+        <v>569.78508565178845</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -20520,7 +20520,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>571.24143928201613</v>
+        <v>569.48094572387822</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -20529,7 +20529,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>570.86958978798668</v>
+        <v>569.22145102062393</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -20538,7 +20538,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>570.28236664647739</v>
+        <v>568.71904748812028</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -20547,7 +20547,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>569.64718278870339</v>
+        <v>568.2625697542602</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -20556,7 +20556,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>569.26611767470354</v>
+        <v>568.052742892423</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -20565,7 +20565,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="1"/>
-        <v>569.07480403227726</v>
+        <v>567.14714522206486</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -20574,7 +20574,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="1"/>
-        <v>568.82417807701563</v>
+        <v>566.37984476971212</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -20583,7 +20583,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>568.71125010747062</v>
+        <v>566.34390030907116</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -20592,7 +20592,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>567.88543703862001</v>
+        <v>565.38213926397088</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -20601,7 +20601,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>567.29613952186401</v>
+        <v>565.136269630637</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -20610,7 +20610,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>566.97781943586529</v>
+        <v>564.25499111203465</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -20619,7 +20619,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>566.61292031105972</v>
+        <v>563.9603113044775</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -20628,7 +20628,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>566.19729983799914</v>
+        <v>563.31700230902425</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -20637,7 +20637,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>565.3177597877808</v>
+        <v>562.42629792368689</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -20646,7 +20646,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>564.97886783359888</v>
+        <v>561.83723461025636</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -20655,7 +20655,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>564.1139728370257</v>
+        <v>561.02371840759929</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -20664,7 +20664,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>564.06507711636709</v>
+        <v>560.85926015241512</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -20673,7 +20673,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="1"/>
-        <v>563.19926073228703</v>
+        <v>560.64528705701775</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -20682,7 +20682,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="1"/>
-        <v>562.27322263959422</v>
+        <v>559.82596387084197</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -20691,7 +20691,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="1"/>
-        <v>561.31089635846718</v>
+        <v>559.14182182474451</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -20700,7 +20700,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="1"/>
-        <v>560.9363864943823</v>
+        <v>559.07914975219023</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -20709,7 +20709,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="1"/>
-        <v>560.57395638516289</v>
+        <v>558.58424745920877</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -20718,7 +20718,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="1"/>
-        <v>560.45768964845422</v>
+        <v>557.95584942283051</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -20727,7 +20727,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="1"/>
-        <v>560.34124084664438</v>
+        <v>557.86247984336546</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -20736,7 +20736,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="1"/>
-        <v>559.35262340823226</v>
+        <v>557.5961045121096</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -20745,7 +20745,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="1"/>
-        <v>558.41978860157269</v>
+        <v>557.32339701311514</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -20754,7 +20754,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="1"/>
-        <v>557.73236797219499</v>
+        <v>556.84074540261622</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -20763,7 +20763,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="1"/>
-        <v>557.66213949172561</v>
+        <v>556.00808554945274</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -20772,7 +20772,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="1"/>
-        <v>556.67604386945493</v>
+        <v>555.33538078351171</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -20781,7 +20781,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="1"/>
-        <v>556.29136954864464</v>
+        <v>555.17721040559184</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -20790,7 +20790,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="1"/>
-        <v>555.63625603567652</v>
+        <v>555.16133111080785</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -20799,7 +20799,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="1"/>
-        <v>555.14356287344003</v>
+        <v>554.60897122657946</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -20808,7 +20808,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="1"/>
-        <v>554.64809297934335</v>
+        <v>554.32463198570088</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -20817,7 +20817,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="1"/>
-        <v>554.04623802167669</v>
+        <v>553.34309938624779</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -20826,7 +20826,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="1"/>
-        <v>553.97158676081096</v>
+        <v>553.16249750271299</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -20835,7 +20835,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="1"/>
-        <v>553.69491358753703</v>
+        <v>552.58585963766814</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -20844,7 +20844,7 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="1"/>
-        <v>553.30932876734198</v>
+        <v>551.87104225149153</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -20853,7 +20853,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="1"/>
-        <v>553.14180287828708</v>
+        <v>551.18993681348343</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -20862,7 +20862,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="1"/>
-        <v>552.36606880866714</v>
+        <v>550.81191995674953</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -20871,7 +20871,7 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="1"/>
-        <v>551.60583696666163</v>
+        <v>549.90703307844853</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -20880,7 +20880,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="1"/>
-        <v>550.71632807785932</v>
+        <v>549.31087535512972</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -20889,7 +20889,7 @@
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="1"/>
-        <v>549.71745271067448</v>
+        <v>548.62202036428141</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -20898,7 +20898,7 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="1"/>
-        <v>548.79751462294223</v>
+        <v>547.90738535155094</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -20907,7 +20907,7 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="1"/>
-        <v>548.28944497765906</v>
+        <v>547.74133473526274</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -20916,7 +20916,7 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="1"/>
-        <v>547.95202648763268</v>
+        <v>547.09818704735198</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -20925,7 +20925,7 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="1"/>
-        <v>547.64604430605891</v>
+        <v>546.87819198272894</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -20934,7 +20934,7 @@
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="1"/>
-        <v>547.04752869606239</v>
+        <v>546.27576589714431</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -20943,7 +20943,7 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="1"/>
-        <v>546.5831593610211</v>
+        <v>545.32080151542766</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -20952,7 +20952,7 @@
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="1"/>
-        <v>545.86450321665666</v>
+        <v>544.58553103908878</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -20961,7 +20961,7 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="1"/>
-        <v>545.63745912882257</v>
+        <v>543.89202655855911</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -20970,7 +20970,7 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="1"/>
-        <v>544.73032647084187</v>
+        <v>543.55058213250777</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -20979,7 +20979,7 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="1"/>
-        <v>544.69485817961527</v>
+        <v>543.38772203282235</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -20988,7 +20988,7 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="1"/>
-        <v>543.83260511356946</v>
+        <v>542.39413614332977</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -20997,7 +20997,7 @@
       </c>
       <c r="B114">
         <f ca="1">B113+0.1*RAND()</f>
-        <v>543.83941573081108</v>
+        <v>542.40423531431759</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -21006,7 +21006,7 @@
       </c>
       <c r="B115">
         <f t="shared" ref="B115:B178" ca="1" si="2">B114+0.1*RAND()</f>
-        <v>543.85349673622545</v>
+        <v>542.49657919465733</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -21015,7 +21015,7 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="2"/>
-        <v>543.87349272331755</v>
+        <v>542.53611736912785</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -21024,7 +21024,7 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="2"/>
-        <v>543.92174177134541</v>
+        <v>542.60676105318259</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -21033,7 +21033,7 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="2"/>
-        <v>543.9504628507309</v>
+        <v>542.61242939889132</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -21042,7 +21042,7 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="2"/>
-        <v>544.00341373805145</v>
+        <v>542.62188860644392</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -21051,7 +21051,7 @@
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="2"/>
-        <v>544.01594294994027</v>
+        <v>542.62489985473508</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -21060,7 +21060,7 @@
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="2"/>
-        <v>544.05483462611676</v>
+        <v>542.65207496081621</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -21069,7 +21069,7 @@
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="2"/>
-        <v>544.12387357418606</v>
+        <v>542.7223824542159</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -21078,7 +21078,7 @@
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="2"/>
-        <v>544.16365832948691</v>
+        <v>542.79969108355533</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -21087,7 +21087,7 @@
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="2"/>
-        <v>544.18849258082651</v>
+        <v>542.81280930225307</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -21096,7 +21096,7 @@
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="2"/>
-        <v>544.2291117319819</v>
+        <v>542.88021480119608</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -21105,7 +21105,7 @@
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="2"/>
-        <v>544.29457928398165</v>
+        <v>542.94991677477901</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -21114,7 +21114,7 @@
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="2"/>
-        <v>544.35755682677984</v>
+        <v>543.03691374070684</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -21123,7 +21123,7 @@
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="2"/>
-        <v>544.44757740201169</v>
+        <v>543.04742446001387</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -21132,7 +21132,7 @@
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="2"/>
-        <v>544.52135335224386</v>
+        <v>543.10644910794133</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -21141,7 +21141,7 @@
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="2"/>
-        <v>544.54132607699114</v>
+        <v>543.12493488268331</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -21150,7 +21150,7 @@
       </c>
       <c r="B131">
         <f t="shared" ca="1" si="2"/>
-        <v>544.63192542294155</v>
+        <v>543.12627892354772</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -21159,7 +21159,7 @@
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="2"/>
-        <v>544.67286198609872</v>
+        <v>543.19504009610239</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -21168,7 +21168,7 @@
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="2"/>
-        <v>544.75080187347032</v>
+        <v>543.23125192591874</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -21177,7 +21177,7 @@
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="2"/>
-        <v>544.81279525761022</v>
+        <v>543.30832062322429</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -21186,7 +21186,7 @@
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="2"/>
-        <v>544.86189072019897</v>
+        <v>543.34626441539729</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -21195,7 +21195,7 @@
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="2"/>
-        <v>544.95707450843008</v>
+        <v>543.41706642322151</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -21204,7 +21204,7 @@
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="2"/>
-        <v>545.04992643488924</v>
+        <v>543.50830594206673</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -21213,7 +21213,7 @@
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="2"/>
-        <v>545.13661265459029</v>
+        <v>543.52536213041628</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -21222,7 +21222,7 @@
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="2"/>
-        <v>545.15954614038446</v>
+        <v>543.5587276181426</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -21231,7 +21231,7 @@
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="2"/>
-        <v>545.16967781866151</v>
+        <v>543.61995141485204</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -21240,7 +21240,7 @@
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="2"/>
-        <v>545.25338124190773</v>
+        <v>543.65164066604052</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -21249,7 +21249,7 @@
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="2"/>
-        <v>545.34380451120614</v>
+        <v>543.6673228825772</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -21258,7 +21258,7 @@
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="2"/>
-        <v>545.3596072739947</v>
+        <v>543.69978235844951</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -21267,7 +21267,7 @@
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="2"/>
-        <v>545.40434940131263</v>
+        <v>543.77283092256869</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -21276,7 +21276,7 @@
       </c>
       <c r="B145">
         <f t="shared" ca="1" si="2"/>
-        <v>545.45891406897567</v>
+        <v>543.80060263792063</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -21285,7 +21285,7 @@
       </c>
       <c r="B146">
         <f t="shared" ca="1" si="2"/>
-        <v>545.54148963368471</v>
+        <v>543.82117005713292</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -21294,7 +21294,7 @@
       </c>
       <c r="B147">
         <f t="shared" ca="1" si="2"/>
-        <v>545.6024935683073</v>
+        <v>543.84315775198468</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -21303,7 +21303,7 @@
       </c>
       <c r="B148">
         <f t="shared" ca="1" si="2"/>
-        <v>545.67706638715538</v>
+        <v>543.93676438442662</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -21312,7 +21312,7 @@
       </c>
       <c r="B149">
         <f t="shared" ca="1" si="2"/>
-        <v>545.74516431705786</v>
+        <v>543.97350912958154</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -21321,7 +21321,7 @@
       </c>
       <c r="B150">
         <f t="shared" ca="1" si="2"/>
-        <v>545.8178912954138</v>
+        <v>543.98125534567828</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -21330,7 +21330,7 @@
       </c>
       <c r="B151">
         <f t="shared" ca="1" si="2"/>
-        <v>545.84651980956664</v>
+        <v>544.07935105639194</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -21339,7 +21339,7 @@
       </c>
       <c r="B152">
         <f t="shared" ca="1" si="2"/>
-        <v>545.88214301994594</v>
+        <v>544.15824726054302</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -21348,7 +21348,7 @@
       </c>
       <c r="B153">
         <f t="shared" ca="1" si="2"/>
-        <v>545.94307601263995</v>
+        <v>544.25693132841877</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -21357,7 +21357,7 @@
       </c>
       <c r="B154">
         <f t="shared" ca="1" si="2"/>
-        <v>546.02806052206324</v>
+        <v>544.27389045614575</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -21366,7 +21366,7 @@
       </c>
       <c r="B155">
         <f t="shared" ca="1" si="2"/>
-        <v>546.03367322412555</v>
+        <v>544.34210481596688</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -21375,7 +21375,7 @@
       </c>
       <c r="B156">
         <f t="shared" ca="1" si="2"/>
-        <v>546.08430806679337</v>
+        <v>544.43042406614336</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -21384,7 +21384,7 @@
       </c>
       <c r="B157">
         <f t="shared" ca="1" si="2"/>
-        <v>546.17868784117672</v>
+        <v>544.49537057754526</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -21393,7 +21393,7 @@
       </c>
       <c r="B158">
         <f t="shared" ca="1" si="2"/>
-        <v>546.20233421019316</v>
+        <v>544.54867153504381</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -21402,7 +21402,7 @@
       </c>
       <c r="B159">
         <f t="shared" ca="1" si="2"/>
-        <v>546.29104815331971</v>
+        <v>544.64236666752606</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -21411,7 +21411,7 @@
       </c>
       <c r="B160">
         <f t="shared" ca="1" si="2"/>
-        <v>546.31690365385157</v>
+        <v>544.66583176199458</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -21420,7 +21420,7 @@
       </c>
       <c r="B161">
         <f t="shared" ca="1" si="2"/>
-        <v>546.33383928423518</v>
+        <v>544.67718560573405</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -21429,7 +21429,7 @@
       </c>
       <c r="B162">
         <f t="shared" ca="1" si="2"/>
-        <v>546.40133112515457</v>
+        <v>544.7501505167171</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -21438,7 +21438,7 @@
       </c>
       <c r="B163">
         <f t="shared" ca="1" si="2"/>
-        <v>546.42444614026294</v>
+        <v>544.80918817244583</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -21447,7 +21447,7 @@
       </c>
       <c r="B164">
         <f t="shared" ca="1" si="2"/>
-        <v>546.46269055811956</v>
+        <v>544.88161933977779</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -21456,7 +21456,7 @@
       </c>
       <c r="B165">
         <f t="shared" ca="1" si="2"/>
-        <v>546.49631364391871</v>
+        <v>544.93054357464246</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -21465,7 +21465,7 @@
       </c>
       <c r="B166">
         <f t="shared" ca="1" si="2"/>
-        <v>546.52390386409775</v>
+        <v>544.93622568945932</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -21474,7 +21474,7 @@
       </c>
       <c r="B167">
         <f t="shared" ca="1" si="2"/>
-        <v>546.60215470499145</v>
+        <v>545.03306493857224</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -21483,7 +21483,7 @@
       </c>
       <c r="B168">
         <f t="shared" ca="1" si="2"/>
-        <v>546.60991581981864</v>
+        <v>545.08228564078763</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -21492,7 +21492,7 @@
       </c>
       <c r="B169">
         <f t="shared" ca="1" si="2"/>
-        <v>546.62821194994115</v>
+        <v>545.1511258973328</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -21501,7 +21501,7 @@
       </c>
       <c r="B170">
         <f t="shared" ca="1" si="2"/>
-        <v>546.6994856941734</v>
+        <v>545.18249683385841</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -21510,7 +21510,7 @@
       </c>
       <c r="B171">
         <f t="shared" ca="1" si="2"/>
-        <v>546.76547153408558</v>
+        <v>545.20749829097895</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -21519,7 +21519,7 @@
       </c>
       <c r="B172">
         <f t="shared" ca="1" si="2"/>
-        <v>546.78871295954229</v>
+        <v>545.29871527440787</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -21528,7 +21528,7 @@
       </c>
       <c r="B173">
         <f t="shared" ca="1" si="2"/>
-        <v>546.82904381247124</v>
+        <v>545.32314985067603</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -21537,7 +21537,7 @@
       </c>
       <c r="B174">
         <f t="shared" ca="1" si="2"/>
-        <v>546.88857503280394</v>
+        <v>545.32484619715194</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -21546,7 +21546,7 @@
       </c>
       <c r="B175">
         <f t="shared" ca="1" si="2"/>
-        <v>546.90234280986169</v>
+        <v>545.36941505098753</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -21555,7 +21555,7 @@
       </c>
       <c r="B176">
         <f t="shared" ca="1" si="2"/>
-        <v>546.93048202811212</v>
+        <v>545.41328182254949</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -21564,7 +21564,7 @@
       </c>
       <c r="B177">
         <f t="shared" ca="1" si="2"/>
-        <v>546.97196296530353</v>
+        <v>545.46114854938628</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -21573,7 +21573,7 @@
       </c>
       <c r="B178">
         <f t="shared" ca="1" si="2"/>
-        <v>547.00542080582409</v>
+        <v>545.51655159098527</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -21582,7 +21582,7 @@
       </c>
       <c r="B179">
         <f t="shared" ref="B179:B242" ca="1" si="3">B178+0.1*RAND()</f>
-        <v>547.10417697079936</v>
+        <v>545.5775532562194</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -21591,7 +21591,7 @@
       </c>
       <c r="B180">
         <f t="shared" ca="1" si="3"/>
-        <v>547.12585594335042</v>
+        <v>545.64010559936833</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -21600,7 +21600,7 @@
       </c>
       <c r="B181">
         <f t="shared" ca="1" si="3"/>
-        <v>547.22070013845894</v>
+        <v>545.708598592474</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -21609,7 +21609,7 @@
       </c>
       <c r="B182">
         <f t="shared" ca="1" si="3"/>
-        <v>547.2298776090895</v>
+        <v>545.79988573636126</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -21618,7 +21618,7 @@
       </c>
       <c r="B183">
         <f t="shared" ca="1" si="3"/>
-        <v>547.23305947327606</v>
+        <v>545.80431780682341</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -21627,7 +21627,7 @@
       </c>
       <c r="B184">
         <f t="shared" ca="1" si="3"/>
-        <v>547.30730467771559</v>
+        <v>545.85877788236473</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -21636,7 +21636,7 @@
       </c>
       <c r="B185">
         <f t="shared" ca="1" si="3"/>
-        <v>547.3179246844004</v>
+        <v>545.87791619112397</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -21645,7 +21645,7 @@
       </c>
       <c r="B186">
         <f t="shared" ca="1" si="3"/>
-        <v>547.37660977893654</v>
+        <v>545.93902195810097</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -21654,7 +21654,7 @@
       </c>
       <c r="B187">
         <f t="shared" ca="1" si="3"/>
-        <v>547.47226462451499</v>
+        <v>546.02871379874193</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -21663,7 +21663,7 @@
       </c>
       <c r="B188">
         <f t="shared" ca="1" si="3"/>
-        <v>547.49619076684166</v>
+        <v>546.0713129459657</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -21672,7 +21672,7 @@
       </c>
       <c r="B189">
         <f t="shared" ca="1" si="3"/>
-        <v>547.50803079466732</v>
+        <v>546.16033196847809</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -21681,7 +21681,7 @@
       </c>
       <c r="B190">
         <f t="shared" ca="1" si="3"/>
-        <v>547.54412366139297</v>
+        <v>546.24061337745673</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -21690,7 +21690,7 @@
       </c>
       <c r="B191">
         <f t="shared" ca="1" si="3"/>
-        <v>547.6374824838756</v>
+        <v>546.25672007690503</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -21699,7 +21699,7 @@
       </c>
       <c r="B192">
         <f t="shared" ca="1" si="3"/>
-        <v>547.72024706949389</v>
+        <v>546.32320957168884</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -21708,7 +21708,7 @@
       </c>
       <c r="B193">
         <f t="shared" ca="1" si="3"/>
-        <v>547.74195329134125</v>
+        <v>546.33242395436719</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -21717,7 +21717,7 @@
       </c>
       <c r="B194">
         <f t="shared" ca="1" si="3"/>
-        <v>547.80962533848708</v>
+        <v>546.33779036531723</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -21726,7 +21726,7 @@
       </c>
       <c r="B195">
         <f t="shared" ca="1" si="3"/>
-        <v>547.83223210926724</v>
+        <v>546.43479156001854</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -21735,7 +21735,7 @@
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="3"/>
-        <v>547.8355116202747</v>
+        <v>546.45040772300058</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -21744,7 +21744,7 @@
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="3"/>
-        <v>547.93474009564784</v>
+        <v>546.50385546954067</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -21753,7 +21753,7 @@
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="3"/>
-        <v>548.02665466058193</v>
+        <v>546.54788947155498</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -21762,7 +21762,7 @@
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="3"/>
-        <v>548.10169276691795</v>
+        <v>546.63054968405106</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -21771,7 +21771,7 @@
       </c>
       <c r="B200">
         <f t="shared" ca="1" si="3"/>
-        <v>548.1844455963701</v>
+        <v>546.69603944907681</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -21780,7 +21780,7 @@
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="3"/>
-        <v>548.22807122168899</v>
+        <v>546.78258861196946</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -21789,7 +21789,7 @@
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="3"/>
-        <v>548.24410486845454</v>
+        <v>546.86781775681288</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -21798,7 +21798,7 @@
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="3"/>
-        <v>548.32697012528695</v>
+        <v>546.95672408638575</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -21807,7 +21807,7 @@
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="3"/>
-        <v>548.37504263714118</v>
+        <v>546.98180931675176</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -21816,7 +21816,7 @@
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="3"/>
-        <v>548.45193826934417</v>
+        <v>547.04249541609954</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -21825,7 +21825,7 @@
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="3"/>
-        <v>548.48454109746854</v>
+        <v>547.1077292962982</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -21834,7 +21834,7 @@
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="3"/>
-        <v>548.55911515907985</v>
+        <v>547.11804963656607</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -21843,7 +21843,7 @@
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="3"/>
-        <v>548.65253932529197</v>
+        <v>547.16201437058908</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -21852,7 +21852,7 @@
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="3"/>
-        <v>548.74213016839133</v>
+        <v>547.24489040570427</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -21861,7 +21861,7 @@
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="3"/>
-        <v>548.78998679108599</v>
+        <v>547.26570836945029</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -21870,7 +21870,7 @@
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="3"/>
-        <v>548.85789644638351</v>
+        <v>547.27105839935564</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -21879,7 +21879,7 @@
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="3"/>
-        <v>548.95377439847448</v>
+        <v>547.3572653799223</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -21888,7 +21888,7 @@
       </c>
       <c r="B213">
         <f t="shared" ca="1" si="3"/>
-        <v>549.04818184854969</v>
+        <v>547.40260582043152</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -21897,7 +21897,7 @@
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="3"/>
-        <v>549.11330401395867</v>
+        <v>547.43807912928025</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -21906,7 +21906,7 @@
       </c>
       <c r="B215">
         <f t="shared" ca="1" si="3"/>
-        <v>549.14718649136273</v>
+        <v>547.47358581575395</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -21915,7 +21915,7 @@
       </c>
       <c r="B216">
         <f t="shared" ca="1" si="3"/>
-        <v>549.2196273478919</v>
+        <v>547.50317266740126</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -21924,7 +21924,7 @@
       </c>
       <c r="B217">
         <f t="shared" ca="1" si="3"/>
-        <v>549.24074978428166</v>
+        <v>547.55920634372251</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -21933,7 +21933,7 @@
       </c>
       <c r="B218">
         <f t="shared" ca="1" si="3"/>
-        <v>549.28913080158259</v>
+        <v>547.63674155725857</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -21942,7 +21942,7 @@
       </c>
       <c r="B219">
         <f t="shared" ca="1" si="3"/>
-        <v>549.35224213681022</v>
+        <v>547.66310226757435</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -21951,7 +21951,7 @@
       </c>
       <c r="B220">
         <f t="shared" ca="1" si="3"/>
-        <v>549.38909216165996</v>
+        <v>547.72924707869367</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -21960,7 +21960,7 @@
       </c>
       <c r="B221">
         <f t="shared" ca="1" si="3"/>
-        <v>549.42892413531683</v>
+        <v>547.80645954676993</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -21969,7 +21969,7 @@
       </c>
       <c r="B222">
         <f t="shared" ca="1" si="3"/>
-        <v>549.44267033135623</v>
+        <v>547.86784722037999</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -21978,7 +21978,7 @@
       </c>
       <c r="B223">
         <f t="shared" ca="1" si="3"/>
-        <v>549.51468114647594</v>
+        <v>547.91646105535392</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -21987,7 +21987,7 @@
       </c>
       <c r="B224">
         <f t="shared" ca="1" si="3"/>
-        <v>549.60524427961832</v>
+        <v>547.91808448904112</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -21996,7 +21996,7 @@
       </c>
       <c r="B225">
         <f t="shared" ca="1" si="3"/>
-        <v>549.63874688989267</v>
+        <v>547.94795675908892</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -22005,7 +22005,7 @@
       </c>
       <c r="B226">
         <f t="shared" ca="1" si="3"/>
-        <v>549.68405779480906</v>
+        <v>547.99855711441603</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -22014,7 +22014,7 @@
       </c>
       <c r="B227">
         <f t="shared" ca="1" si="3"/>
-        <v>549.72158972778664</v>
+        <v>548.05730112381343</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -22023,7 +22023,7 @@
       </c>
       <c r="B228">
         <f t="shared" ca="1" si="3"/>
-        <v>549.78705186529305</v>
+        <v>548.11764929905542</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -22032,7 +22032,7 @@
       </c>
       <c r="B229">
         <f t="shared" ca="1" si="3"/>
-        <v>549.83372437175342</v>
+        <v>548.1422198094433</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -22041,7 +22041,7 @@
       </c>
       <c r="B230">
         <f t="shared" ca="1" si="3"/>
-        <v>549.85675281118574</v>
+        <v>548.23037475047272</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -22050,7 +22050,7 @@
       </c>
       <c r="B231">
         <f t="shared" ca="1" si="3"/>
-        <v>549.9182613047949</v>
+        <v>548.23304843498215</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -22059,7 +22059,7 @@
       </c>
       <c r="B232">
         <f t="shared" ca="1" si="3"/>
-        <v>549.99140356497207</v>
+        <v>548.28258005846089</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -22068,7 +22068,7 @@
       </c>
       <c r="B233">
         <f t="shared" ca="1" si="3"/>
-        <v>550.05374868904994</v>
+        <v>548.3269687157117</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -22077,7 +22077,7 @@
       </c>
       <c r="B234">
         <f t="shared" ca="1" si="3"/>
-        <v>550.07077532959056</v>
+        <v>548.41833644836095</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -22086,7 +22086,7 @@
       </c>
       <c r="B235">
         <f t="shared" ca="1" si="3"/>
-        <v>550.07386603251905</v>
+        <v>548.51661118292657</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -22095,7 +22095,7 @@
       </c>
       <c r="B236">
         <f t="shared" ca="1" si="3"/>
-        <v>550.10599922912365</v>
+        <v>548.54024219797395</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -22104,7 +22104,7 @@
       </c>
       <c r="B237">
         <f t="shared" ca="1" si="3"/>
-        <v>550.1911917904165</v>
+        <v>548.54518001163103</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -22113,7 +22113,7 @@
       </c>
       <c r="B238">
         <f t="shared" ca="1" si="3"/>
-        <v>550.24910097003124</v>
+        <v>548.63650690191184</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -22122,7 +22122,7 @@
       </c>
       <c r="B239">
         <f t="shared" ca="1" si="3"/>
-        <v>550.33847332969242</v>
+        <v>548.69936969537832</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -22131,7 +22131,7 @@
       </c>
       <c r="B240">
         <f t="shared" ca="1" si="3"/>
-        <v>550.36719486890263</v>
+        <v>548.71371293743425</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -22140,7 +22140,7 @@
       </c>
       <c r="B241">
         <f t="shared" ca="1" si="3"/>
-        <v>550.40211816984367</v>
+        <v>548.73056428245388</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -22149,7 +22149,7 @@
       </c>
       <c r="B242">
         <f t="shared" ca="1" si="3"/>
-        <v>550.48785024684275</v>
+        <v>548.80292770984238</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -22158,7 +22158,7 @@
       </c>
       <c r="B243">
         <f t="shared" ref="B243:B306" ca="1" si="4">B242+0.1*RAND()</f>
-        <v>550.57022836631336</v>
+        <v>548.89704702512063</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -22167,7 +22167,7 @@
       </c>
       <c r="B244">
         <f t="shared" ca="1" si="4"/>
-        <v>550.60950529834577</v>
+        <v>548.95478858713557</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -22176,7 +22176,7 @@
       </c>
       <c r="B245">
         <f t="shared" ca="1" si="4"/>
-        <v>550.69441916072299</v>
+        <v>548.98370709568826</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -22185,7 +22185,7 @@
       </c>
       <c r="B246">
         <f t="shared" ca="1" si="4"/>
-        <v>550.72261350518193</v>
+        <v>549.00881834601353</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -22194,7 +22194,7 @@
       </c>
       <c r="B247">
         <f t="shared" ca="1" si="4"/>
-        <v>550.78830763126552</v>
+        <v>549.05355102138594</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -22203,7 +22203,7 @@
       </c>
       <c r="B248">
         <f t="shared" ca="1" si="4"/>
-        <v>550.82410250001465</v>
+        <v>549.1375363339929</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -22212,7 +22212,7 @@
       </c>
       <c r="B249">
         <f t="shared" ca="1" si="4"/>
-        <v>550.84765251770955</v>
+        <v>549.18392737055888</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -22221,7 +22221,7 @@
       </c>
       <c r="B250">
         <f t="shared" ca="1" si="4"/>
-        <v>550.86455481731014</v>
+        <v>549.27076509482436</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -22230,7 +22230,7 @@
       </c>
       <c r="B251">
         <f t="shared" ca="1" si="4"/>
-        <v>550.94413600871917</v>
+        <v>549.30409238094148</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -22239,7 +22239,7 @@
       </c>
       <c r="B252">
         <f t="shared" ca="1" si="4"/>
-        <v>550.99165504588302</v>
+        <v>549.32946898745308</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -22248,7 +22248,7 @@
       </c>
       <c r="B253">
         <f t="shared" ca="1" si="4"/>
-        <v>551.05478561208042</v>
+        <v>549.38034121000021</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -22257,7 +22257,7 @@
       </c>
       <c r="B254">
         <f t="shared" ca="1" si="4"/>
-        <v>551.0607911361576</v>
+        <v>549.40299960583468</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -22266,7 +22266,7 @@
       </c>
       <c r="B255">
         <f t="shared" ca="1" si="4"/>
-        <v>551.11152455412844</v>
+        <v>549.45336473117925</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -22275,7 +22275,7 @@
       </c>
       <c r="B256">
         <f t="shared" ca="1" si="4"/>
-        <v>551.17998391693936</v>
+        <v>549.52405106317667</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -22284,7 +22284,7 @@
       </c>
       <c r="B257">
         <f t="shared" ca="1" si="4"/>
-        <v>551.23231802674434</v>
+        <v>549.54767130036032</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -22293,7 +22293,7 @@
       </c>
       <c r="B258">
         <f t="shared" ca="1" si="4"/>
-        <v>551.30402848500671</v>
+        <v>549.55454783570917</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -22302,7 +22302,7 @@
       </c>
       <c r="B259">
         <f t="shared" ca="1" si="4"/>
-        <v>551.37847499263921</v>
+        <v>549.64679784121324</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -22311,7 +22311,7 @@
       </c>
       <c r="B260">
         <f t="shared" ca="1" si="4"/>
-        <v>551.42728009482596</v>
+        <v>549.70631988099012</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -22320,7 +22320,7 @@
       </c>
       <c r="B261">
         <f t="shared" ca="1" si="4"/>
-        <v>551.518478367748</v>
+        <v>549.73942500743465</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -22329,7 +22329,7 @@
       </c>
       <c r="B262">
         <f t="shared" ca="1" si="4"/>
-        <v>551.60484307592526</v>
+        <v>549.82284287621826</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
@@ -22338,7 +22338,7 @@
       </c>
       <c r="B263">
         <f t="shared" ca="1" si="4"/>
-        <v>551.70237101064356</v>
+        <v>549.88615611008413</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -22347,7 +22347,7 @@
       </c>
       <c r="B264">
         <f t="shared" ca="1" si="4"/>
-        <v>551.75479102696704</v>
+        <v>549.93273870543749</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -22356,7 +22356,7 @@
       </c>
       <c r="B265">
         <f t="shared" ca="1" si="4"/>
-        <v>551.77208669948413</v>
+        <v>549.98762380418771</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -22365,7 +22365,7 @@
       </c>
       <c r="B266">
         <f t="shared" ca="1" si="4"/>
-        <v>551.79360208723358</v>
+        <v>550.0180223678417</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
@@ -22374,7 +22374,7 @@
       </c>
       <c r="B267">
         <f t="shared" ca="1" si="4"/>
-        <v>551.84167362645144</v>
+        <v>550.11078780276807</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -22383,7 +22383,7 @@
       </c>
       <c r="B268">
         <f t="shared" ca="1" si="4"/>
-        <v>551.87895645534161</v>
+        <v>550.20366755511441</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
@@ -22392,7 +22392,7 @@
       </c>
       <c r="B269">
         <f t="shared" ca="1" si="4"/>
-        <v>551.94491496899366</v>
+        <v>550.26471274934772</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
@@ -22401,7 +22401,7 @@
       </c>
       <c r="B270">
         <f t="shared" ca="1" si="4"/>
-        <v>551.96243715689036</v>
+        <v>550.33882471147444</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -22410,7 +22410,7 @@
       </c>
       <c r="B271">
         <f t="shared" ca="1" si="4"/>
-        <v>551.97194900873274</v>
+        <v>550.40297455068662</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
@@ -22419,7 +22419,7 @@
       </c>
       <c r="B272">
         <f t="shared" ca="1" si="4"/>
-        <v>551.99612048959273</v>
+        <v>550.46170502145071</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
@@ -22428,7 +22428,7 @@
       </c>
       <c r="B273">
         <f t="shared" ca="1" si="4"/>
-        <v>552.07049231104611</v>
+        <v>550.52224847417699</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -22437,7 +22437,7 @@
       </c>
       <c r="B274">
         <f t="shared" ca="1" si="4"/>
-        <v>552.09065868857317</v>
+        <v>550.58621497237414</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -22446,7 +22446,7 @@
       </c>
       <c r="B275">
         <f t="shared" ca="1" si="4"/>
-        <v>552.17064116660265</v>
+        <v>550.62142877876715</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -22455,7 +22455,7 @@
       </c>
       <c r="B276">
         <f t="shared" ca="1" si="4"/>
-        <v>552.2404998319829</v>
+        <v>550.64523775828422</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -22464,7 +22464,7 @@
       </c>
       <c r="B277">
         <f t="shared" ca="1" si="4"/>
-        <v>552.33088647430861</v>
+        <v>550.67864228352823</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -22473,7 +22473,7 @@
       </c>
       <c r="B278">
         <f t="shared" ca="1" si="4"/>
-        <v>552.35512614237939</v>
+        <v>550.76234906957154</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
@@ -22482,7 +22482,7 @@
       </c>
       <c r="B279">
         <f t="shared" ca="1" si="4"/>
-        <v>552.45221849167342</v>
+        <v>550.84039581109528</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -22491,7 +22491,7 @@
       </c>
       <c r="B280">
         <f t="shared" ca="1" si="4"/>
-        <v>552.48057032525548</v>
+        <v>550.86446739730729</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
@@ -22500,7 +22500,7 @@
       </c>
       <c r="B281">
         <f t="shared" ca="1" si="4"/>
-        <v>552.57064448410563</v>
+        <v>550.95653132327357</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
@@ -22509,7 +22509,7 @@
       </c>
       <c r="B282">
         <f t="shared" ca="1" si="4"/>
-        <v>552.5708383575942</v>
+        <v>551.03284425955167</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -22518,7 +22518,7 @@
       </c>
       <c r="B283">
         <f t="shared" ca="1" si="4"/>
-        <v>552.63193692551738</v>
+        <v>551.08365662271888</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
@@ -22527,7 +22527,7 @@
       </c>
       <c r="B284">
         <f t="shared" ca="1" si="4"/>
-        <v>552.64806791416243</v>
+        <v>551.14541168635333</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -22536,7 +22536,7 @@
       </c>
       <c r="B285">
         <f t="shared" ca="1" si="4"/>
-        <v>552.69333059327903</v>
+        <v>551.1726496999579</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -22545,7 +22545,7 @@
       </c>
       <c r="B286">
         <f t="shared" ca="1" si="4"/>
-        <v>552.78669267038504</v>
+        <v>551.25257174301771</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
@@ -22554,7 +22554,7 @@
       </c>
       <c r="B287">
         <f t="shared" ca="1" si="4"/>
-        <v>552.85947366810774</v>
+        <v>551.25384101514601</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
@@ -22563,7 +22563,7 @@
       </c>
       <c r="B288">
         <f t="shared" ca="1" si="4"/>
-        <v>552.86215576636585</v>
+        <v>551.32640106887925</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -22572,7 +22572,7 @@
       </c>
       <c r="B289">
         <f t="shared" ca="1" si="4"/>
-        <v>552.86242941031765</v>
+        <v>551.40823469419161</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
@@ -22581,7 +22581,7 @@
       </c>
       <c r="B290">
         <f t="shared" ca="1" si="4"/>
-        <v>552.86894606112708</v>
+        <v>551.4936553520555</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
@@ -22590,7 +22590,7 @@
       </c>
       <c r="B291">
         <f t="shared" ca="1" si="4"/>
-        <v>552.88419533659635</v>
+        <v>551.54473771543962</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -22599,7 +22599,7 @@
       </c>
       <c r="B292">
         <f t="shared" ca="1" si="4"/>
-        <v>552.93109153711703</v>
+        <v>551.58430243662053</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
@@ -22608,7 +22608,7 @@
       </c>
       <c r="B293">
         <f t="shared" ca="1" si="4"/>
-        <v>552.99402450446769</v>
+        <v>551.58695849617607</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
@@ -22617,7 +22617,7 @@
       </c>
       <c r="B294">
         <f t="shared" ca="1" si="4"/>
-        <v>553.04781638961799</v>
+        <v>551.58905234704014</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -22626,7 +22626,7 @@
       </c>
       <c r="B295">
         <f t="shared" ca="1" si="4"/>
-        <v>553.14197385738362</v>
+        <v>551.60054750168661</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
@@ -22635,7 +22635,7 @@
       </c>
       <c r="B296">
         <f t="shared" ca="1" si="4"/>
-        <v>553.16213328058177</v>
+        <v>551.60569993994318</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -22644,7 +22644,7 @@
       </c>
       <c r="B297">
         <f t="shared" ca="1" si="4"/>
-        <v>553.19218234047696</v>
+        <v>551.66515256559387</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -22653,7 +22653,7 @@
       </c>
       <c r="B298">
         <f t="shared" ca="1" si="4"/>
-        <v>553.20668493010601</v>
+        <v>551.75595701864643</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -22662,7 +22662,7 @@
       </c>
       <c r="B299">
         <f t="shared" ca="1" si="4"/>
-        <v>553.28364798882797</v>
+        <v>551.84362217575381</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -22671,7 +22671,7 @@
       </c>
       <c r="B300">
         <f t="shared" ca="1" si="4"/>
-        <v>553.35376044545842</v>
+        <v>551.87474783372897</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -22680,7 +22680,7 @@
       </c>
       <c r="B301">
         <f t="shared" ca="1" si="4"/>
-        <v>553.42182616154616</v>
+        <v>551.87995014784201</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -22689,7 +22689,7 @@
       </c>
       <c r="B302">
         <f t="shared" ca="1" si="4"/>
-        <v>553.46602416886265</v>
+        <v>551.91195019394945</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -22698,7 +22698,7 @@
       </c>
       <c r="B303">
         <f t="shared" ca="1" si="4"/>
-        <v>553.4736657746729</v>
+        <v>551.92594662515114</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -22707,7 +22707,7 @@
       </c>
       <c r="B304">
         <f t="shared" ca="1" si="4"/>
-        <v>553.52258444871563</v>
+        <v>552.0252614813902</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -22716,7 +22716,7 @@
       </c>
       <c r="B305">
         <f t="shared" ca="1" si="4"/>
-        <v>553.54348138785895</v>
+        <v>552.09555240880616</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -22725,7 +22725,7 @@
       </c>
       <c r="B306">
         <f t="shared" ca="1" si="4"/>
-        <v>553.61477398831698</v>
+        <v>552.13801729075635</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -22734,7 +22734,7 @@
       </c>
       <c r="B307">
         <f t="shared" ref="B307:B370" ca="1" si="5">B306+0.1*RAND()</f>
-        <v>553.62782594725149</v>
+        <v>552.14159163803004</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -22743,7 +22743,7 @@
       </c>
       <c r="B308">
         <f t="shared" ca="1" si="5"/>
-        <v>553.63357858837844</v>
+        <v>552.17401328094786</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
@@ -22752,7 +22752,7 @@
       </c>
       <c r="B309">
         <f t="shared" ca="1" si="5"/>
-        <v>553.65252510483413</v>
+        <v>552.18600994732628</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -22761,7 +22761,7 @@
       </c>
       <c r="B310">
         <f t="shared" ca="1" si="5"/>
-        <v>553.7096097764869</v>
+        <v>552.26728032569565</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
@@ -22770,7 +22770,7 @@
       </c>
       <c r="B311">
         <f t="shared" ca="1" si="5"/>
-        <v>553.75235391455419</v>
+        <v>552.32066000836778</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -22779,7 +22779,7 @@
       </c>
       <c r="B312">
         <f t="shared" ca="1" si="5"/>
-        <v>553.81761400017001</v>
+        <v>552.41490818675982</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -22788,7 +22788,7 @@
       </c>
       <c r="B313">
         <f t="shared" ca="1" si="5"/>
-        <v>553.89300255822832</v>
+        <v>552.48120764713758</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
@@ -22797,7 +22797,7 @@
       </c>
       <c r="B314">
         <f t="shared" ca="1" si="5"/>
-        <v>553.94833011022683</v>
+        <v>552.49895961229288</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
@@ -22806,7 +22806,7 @@
       </c>
       <c r="B315">
         <f t="shared" ca="1" si="5"/>
-        <v>554.01350993982135</v>
+        <v>552.53448529980028</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -22815,7 +22815,7 @@
       </c>
       <c r="B316">
         <f t="shared" ca="1" si="5"/>
-        <v>554.06213166160649</v>
+        <v>552.58386127524091</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
@@ -22824,7 +22824,7 @@
       </c>
       <c r="B317">
         <f t="shared" ca="1" si="5"/>
-        <v>554.12508334557629</v>
+        <v>552.61677630084819</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
@@ -22833,7 +22833,7 @@
       </c>
       <c r="B318">
         <f t="shared" ca="1" si="5"/>
-        <v>554.18626744945345</v>
+        <v>552.64559523877438</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -22842,7 +22842,7 @@
       </c>
       <c r="B319">
         <f t="shared" ca="1" si="5"/>
-        <v>554.24512393562441</v>
+        <v>552.70253371828653</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
@@ -22851,7 +22851,7 @@
       </c>
       <c r="B320">
         <f t="shared" ca="1" si="5"/>
-        <v>554.24916694127819</v>
+        <v>552.73203068996384</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -22860,7 +22860,7 @@
       </c>
       <c r="B321">
         <f t="shared" ca="1" si="5"/>
-        <v>554.28588491661355</v>
+        <v>552.73726468869575</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -22869,7 +22869,7 @@
       </c>
       <c r="B322">
         <f t="shared" ca="1" si="5"/>
-        <v>554.33435890988824</v>
+        <v>552.76148342843157</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -22878,7 +22878,7 @@
       </c>
       <c r="B323">
         <f t="shared" ca="1" si="5"/>
-        <v>554.3449737314404</v>
+        <v>552.82227187432829</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -22887,7 +22887,7 @@
       </c>
       <c r="B324">
         <f t="shared" ca="1" si="5"/>
-        <v>554.38815988779106</v>
+        <v>552.86755618003156</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -22896,7 +22896,7 @@
       </c>
       <c r="B325">
         <f t="shared" ca="1" si="5"/>
-        <v>554.41065290458232</v>
+        <v>552.93084550910953</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
@@ -22905,7 +22905,7 @@
       </c>
       <c r="B326">
         <f t="shared" ca="1" si="5"/>
-        <v>554.50868422585279</v>
+        <v>553.0119263177952</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
@@ -22914,7 +22914,7 @@
       </c>
       <c r="B327">
         <f t="shared" ca="1" si="5"/>
-        <v>554.52359394912924</v>
+        <v>553.09708062138873</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -22923,7 +22923,7 @@
       </c>
       <c r="B328">
         <f t="shared" ca="1" si="5"/>
-        <v>554.54620659879492</v>
+        <v>553.15752512268909</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
@@ -22932,7 +22932,7 @@
       </c>
       <c r="B329">
         <f t="shared" ca="1" si="5"/>
-        <v>554.5998041858453</v>
+        <v>553.21507146683314</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -22941,7 +22941,7 @@
       </c>
       <c r="B330">
         <f t="shared" ca="1" si="5"/>
-        <v>554.67718474830338</v>
+        <v>553.29740106970644</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -22950,7 +22950,7 @@
       </c>
       <c r="B331">
         <f t="shared" ca="1" si="5"/>
-        <v>554.69282936006721</v>
+        <v>553.34261673302228</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -22959,7 +22959,7 @@
       </c>
       <c r="B332">
         <f t="shared" ca="1" si="5"/>
-        <v>554.78433153034496</v>
+        <v>553.42435158904061</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -22968,7 +22968,7 @@
       </c>
       <c r="B333">
         <f t="shared" ca="1" si="5"/>
-        <v>554.85380135840512</v>
+        <v>553.51575729180547</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -22977,7 +22977,7 @@
       </c>
       <c r="B334">
         <f t="shared" ca="1" si="5"/>
-        <v>554.90530025326541</v>
+        <v>553.54691157544346</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
@@ -22986,7 +22986,7 @@
       </c>
       <c r="B335">
         <f t="shared" ca="1" si="5"/>
-        <v>554.98302883203689</v>
+        <v>553.62446731713624</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
@@ -22995,7 +22995,7 @@
       </c>
       <c r="B336">
         <f t="shared" ca="1" si="5"/>
-        <v>554.98325355099837</v>
+        <v>553.64235937935609</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -23004,7 +23004,7 @@
       </c>
       <c r="B337">
         <f t="shared" ca="1" si="5"/>
-        <v>555.01951589410282</v>
+        <v>553.6556225826339</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
@@ -23013,7 +23013,7 @@
       </c>
       <c r="B338">
         <f t="shared" ca="1" si="5"/>
-        <v>555.09802614211753</v>
+        <v>553.70056025713268</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
@@ -23022,7 +23022,7 @@
       </c>
       <c r="B339">
         <f t="shared" ca="1" si="5"/>
-        <v>555.15533709978251</v>
+        <v>553.76206353927444</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -23031,7 +23031,7 @@
       </c>
       <c r="B340">
         <f t="shared" ca="1" si="5"/>
-        <v>555.18485963713772</v>
+        <v>553.83205749233741</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
@@ -23040,7 +23040,7 @@
       </c>
       <c r="B341">
         <f t="shared" ca="1" si="5"/>
-        <v>555.2639418587172</v>
+        <v>553.88295461195264</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
@@ -23049,7 +23049,7 @@
       </c>
       <c r="B342">
         <f t="shared" ca="1" si="5"/>
-        <v>555.33476349258149</v>
+        <v>553.94691905231048</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -23058,7 +23058,7 @@
       </c>
       <c r="B343">
         <f t="shared" ca="1" si="5"/>
-        <v>555.36872159706638</v>
+        <v>553.98465160898229</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
@@ -23067,7 +23067,7 @@
       </c>
       <c r="B344">
         <f t="shared" ca="1" si="5"/>
-        <v>555.42963702390796</v>
+        <v>553.99906594193897</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
@@ -23076,7 +23076,7 @@
       </c>
       <c r="B345">
         <f t="shared" ca="1" si="5"/>
-        <v>555.51897308195385</v>
+        <v>554.08055686271882</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -23085,7 +23085,7 @@
       </c>
       <c r="B346">
         <f t="shared" ca="1" si="5"/>
-        <v>555.55920625198178</v>
+        <v>554.15391208127789</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
@@ -23094,7 +23094,7 @@
       </c>
       <c r="B347">
         <f t="shared" ca="1" si="5"/>
-        <v>555.55977287558142</v>
+        <v>554.2146463915974</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
@@ -23103,7 +23103,7 @@
       </c>
       <c r="B348">
         <f t="shared" ca="1" si="5"/>
-        <v>555.59659042430462</v>
+        <v>554.22051377030004</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -23112,7 +23112,7 @@
       </c>
       <c r="B349">
         <f t="shared" ca="1" si="5"/>
-        <v>555.68662362800194</v>
+        <v>554.31482536587043</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
@@ -23121,7 +23121,7 @@
       </c>
       <c r="B350">
         <f t="shared" ca="1" si="5"/>
-        <v>555.76528654258493</v>
+        <v>554.38104697491667</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
@@ -23130,7 +23130,7 @@
       </c>
       <c r="B351">
         <f t="shared" ca="1" si="5"/>
-        <v>555.84038393221647</v>
+        <v>554.48077732368313</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -23139,7 +23139,7 @@
       </c>
       <c r="B352">
         <f t="shared" ca="1" si="5"/>
-        <v>555.84123774172213</v>
+        <v>554.54298569489868</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
@@ -23148,7 +23148,7 @@
       </c>
       <c r="B353">
         <f t="shared" ca="1" si="5"/>
-        <v>555.86958645903871</v>
+        <v>554.58342051052944</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
@@ -23157,7 +23157,7 @@
       </c>
       <c r="B354">
         <f t="shared" ca="1" si="5"/>
-        <v>555.91391809225479</v>
+        <v>554.68235461735401</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -23166,7 +23166,7 @@
       </c>
       <c r="B355">
         <f t="shared" ca="1" si="5"/>
-        <v>555.96289688126058</v>
+        <v>554.72721854432245</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
@@ -23175,7 +23175,7 @@
       </c>
       <c r="B356">
         <f t="shared" ca="1" si="5"/>
-        <v>555.99943180186528</v>
+        <v>554.76377785908267</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
@@ -23184,7 +23184,7 @@
       </c>
       <c r="B357">
         <f t="shared" ca="1" si="5"/>
-        <v>556.05072196941285</v>
+        <v>554.8574827233698</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -23193,7 +23193,7 @@
       </c>
       <c r="B358">
         <f t="shared" ca="1" si="5"/>
-        <v>556.09431688372877</v>
+        <v>554.94143030026191</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
@@ -23202,7 +23202,7 @@
       </c>
       <c r="B359">
         <f t="shared" ca="1" si="5"/>
-        <v>556.16500002592932</v>
+        <v>555.00696425216518</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
@@ -23211,7 +23211,7 @@
       </c>
       <c r="B360">
         <f t="shared" ca="1" si="5"/>
-        <v>556.25839477183604</v>
+        <v>555.02747168159578</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -23220,7 +23220,7 @@
       </c>
       <c r="B361">
         <f t="shared" ca="1" si="5"/>
-        <v>556.28087693876353</v>
+        <v>555.06978777861298</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
@@ -23229,7 +23229,7 @@
       </c>
       <c r="B362">
         <f t="shared" ca="1" si="5"/>
-        <v>556.3774696775298</v>
+        <v>555.09151984360972</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
@@ -23238,7 +23238,7 @@
       </c>
       <c r="B363">
         <f t="shared" ca="1" si="5"/>
-        <v>556.40323161455194</v>
+        <v>555.18396003301996</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -23247,7 +23247,7 @@
       </c>
       <c r="B364">
         <f t="shared" ca="1" si="5"/>
-        <v>556.43808919529488</v>
+        <v>555.18746433849128</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
@@ -23256,7 +23256,7 @@
       </c>
       <c r="B365">
         <f t="shared" ca="1" si="5"/>
-        <v>556.46213683521466</v>
+        <v>555.20344463653669</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
@@ -23265,7 +23265,7 @@
       </c>
       <c r="B366">
         <f t="shared" ca="1" si="5"/>
-        <v>556.55847910662794</v>
+        <v>555.20838021659972</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -23274,7 +23274,7 @@
       </c>
       <c r="B367">
         <f t="shared" ca="1" si="5"/>
-        <v>556.57989036646347</v>
+        <v>555.25772742796096</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
@@ -23283,7 +23283,7 @@
       </c>
       <c r="B368">
         <f t="shared" ca="1" si="5"/>
-        <v>556.59974092504092</v>
+        <v>555.31506948477295</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
@@ -23292,7 +23292,7 @@
       </c>
       <c r="B369">
         <f t="shared" ca="1" si="5"/>
-        <v>556.61872295727028</v>
+        <v>555.33666396353874</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -23301,7 +23301,7 @@
       </c>
       <c r="B370">
         <f t="shared" ca="1" si="5"/>
-        <v>556.71523433275127</v>
+        <v>555.43206520762794</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
@@ -23310,7 +23310,7 @@
       </c>
       <c r="B371">
         <f t="shared" ref="B371:B402" ca="1" si="6">B370+0.1*RAND()</f>
-        <v>556.73058236949396</v>
+        <v>555.51707018998434</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -23319,7 +23319,7 @@
       </c>
       <c r="B372">
         <f t="shared" ca="1" si="6"/>
-        <v>556.79424818192967</v>
+        <v>555.55053331555143</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -23328,7 +23328,7 @@
       </c>
       <c r="B373">
         <f t="shared" ca="1" si="6"/>
-        <v>556.84400185867457</v>
+        <v>555.59470319469244</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
@@ -23337,7 +23337,7 @@
       </c>
       <c r="B374">
         <f t="shared" ca="1" si="6"/>
-        <v>556.86462163200395</v>
+        <v>555.63064971069537</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -23346,7 +23346,7 @@
       </c>
       <c r="B375">
         <f t="shared" ca="1" si="6"/>
-        <v>556.92325890052848</v>
+        <v>555.63318674864149</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -23355,7 +23355,7 @@
       </c>
       <c r="B376">
         <f t="shared" ca="1" si="6"/>
-        <v>556.93887951526051</v>
+        <v>555.67766654548245</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
@@ -23364,7 +23364,7 @@
       </c>
       <c r="B377">
         <f t="shared" ca="1" si="6"/>
-        <v>556.96300958209224</v>
+        <v>555.70167951458461</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
@@ -23373,7 +23373,7 @@
       </c>
       <c r="B378">
         <f t="shared" ca="1" si="6"/>
-        <v>556.99286738604985</v>
+        <v>555.73732947342069</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -23382,7 +23382,7 @@
       </c>
       <c r="B379">
         <f t="shared" ca="1" si="6"/>
-        <v>557.02174921899837</v>
+        <v>555.81451193576424</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
@@ -23391,7 +23391,7 @@
       </c>
       <c r="B380">
         <f t="shared" ca="1" si="6"/>
-        <v>557.07963786913967</v>
+        <v>555.87916497856008</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
@@ -23400,7 +23400,7 @@
       </c>
       <c r="B381">
         <f t="shared" ca="1" si="6"/>
-        <v>557.08127927899375</v>
+        <v>555.9228650509308</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -23409,7 +23409,7 @@
       </c>
       <c r="B382">
         <f t="shared" ca="1" si="6"/>
-        <v>557.15729657242605</v>
+        <v>555.95813404345813</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
@@ -23418,7 +23418,7 @@
       </c>
       <c r="B383">
         <f t="shared" ca="1" si="6"/>
-        <v>557.17415156416007</v>
+        <v>556.04062711813765</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
@@ -23427,7 +23427,7 @@
       </c>
       <c r="B384">
         <f t="shared" ca="1" si="6"/>
-        <v>557.27256559477155</v>
+        <v>556.09530573906397</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -23436,7 +23436,7 @@
       </c>
       <c r="B385">
         <f t="shared" ca="1" si="6"/>
-        <v>557.34821587060367</v>
+        <v>556.1515438445881</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
@@ -23445,7 +23445,7 @@
       </c>
       <c r="B386">
         <f t="shared" ca="1" si="6"/>
-        <v>557.39694822998877</v>
+        <v>556.24493074015231</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
@@ -23454,7 +23454,7 @@
       </c>
       <c r="B387">
         <f t="shared" ca="1" si="6"/>
-        <v>557.46910087758067</v>
+        <v>556.31270267935611</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -23463,7 +23463,7 @@
       </c>
       <c r="B388">
         <f t="shared" ca="1" si="6"/>
-        <v>557.51795716151071</v>
+        <v>556.3994491546415</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
@@ -23472,7 +23472,7 @@
       </c>
       <c r="B389">
         <f t="shared" ca="1" si="6"/>
-        <v>557.55578136871895</v>
+        <v>556.40751516088574</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
@@ -23481,7 +23481,7 @@
       </c>
       <c r="B390">
         <f t="shared" ca="1" si="6"/>
-        <v>557.55993090254049</v>
+        <v>556.48650422140997</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -23490,7 +23490,7 @@
       </c>
       <c r="B391">
         <f t="shared" ca="1" si="6"/>
-        <v>557.56926156632767</v>
+        <v>556.53484592641803</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
@@ -23499,7 +23499,7 @@
       </c>
       <c r="B392">
         <f t="shared" ca="1" si="6"/>
-        <v>557.57530746739474</v>
+        <v>556.54657422622449</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
@@ -23508,7 +23508,7 @@
       </c>
       <c r="B393">
         <f t="shared" ca="1" si="6"/>
-        <v>557.65981485792997</v>
+        <v>556.60352327914381</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -23517,7 +23517,7 @@
       </c>
       <c r="B394">
         <f t="shared" ca="1" si="6"/>
-        <v>557.69352677208349</v>
+        <v>556.65220921529544</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
@@ -23526,7 +23526,7 @@
       </c>
       <c r="B395">
         <f t="shared" ca="1" si="6"/>
-        <v>557.75552189355926</v>
+        <v>556.71808311932205</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
@@ -23535,7 +23535,7 @@
       </c>
       <c r="B396">
         <f t="shared" ca="1" si="6"/>
-        <v>557.79436275367766</v>
+        <v>556.79070233791163</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -23544,7 +23544,7 @@
       </c>
       <c r="B397">
         <f t="shared" ca="1" si="6"/>
-        <v>557.86083643341772</v>
+        <v>556.85208146472951</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
@@ -23553,7 +23553,7 @@
       </c>
       <c r="B398">
         <f t="shared" ca="1" si="6"/>
-        <v>557.8985840148697</v>
+        <v>556.87910807846356</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
@@ -23562,7 +23562,7 @@
       </c>
       <c r="B399">
         <f t="shared" ca="1" si="6"/>
-        <v>557.91060260077904</v>
+        <v>556.88121950308607</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -23571,7 +23571,7 @@
       </c>
       <c r="B400">
         <f t="shared" ca="1" si="6"/>
-        <v>557.94737999531174</v>
+        <v>556.946909469753</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
@@ -23580,7 +23580,7 @@
       </c>
       <c r="B401">
         <f t="shared" ca="1" si="6"/>
-        <v>557.9994663028275</v>
+        <v>557.00043422138492</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
@@ -23589,7 +23589,7 @@
       </c>
       <c r="B402">
         <f t="shared" ca="1" si="6"/>
-        <v>558.0814247879506</v>
+        <v>557.02206782482301</v>
       </c>
     </row>
   </sheetData>
@@ -24033,7 +24033,7 @@
   <dimension ref="A1:B502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E390" sqref="E390"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed blackout instability. Checked stability for unplanned disconnect, island-grid connect, and blackout
</commit_message>
<xml_diff>
--- a/CART dependencies/Microgrid_cmd.xlsx
+++ b/CART dependencies/Microgrid_cmd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\FC Microgrid\CART dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BA3D5D-98FE-4051-BD5C-7A8BD6F8AC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB39E6-E2BF-499D-96D6-A1B442545FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11550" windowHeight="10440" xr2:uid="{B24A82DE-2B79-4981-9B7A-F7C055D78750}"/>
   </bookViews>
   <sheets>
     <sheet name="WTGmode" sheetId="13" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19989,7 +19989,7 @@
       </c>
       <c r="B2">
         <f ca="1">575+0.5*RAND()</f>
-        <v>575.07947980138613</v>
+        <v>575.13503831522496</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -19998,7 +19998,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B52" ca="1" si="0">575+0.5*RAND()</f>
-        <v>575.0990236261639</v>
+        <v>575.31509101587631</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20007,7 +20007,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>575.14098195430654</v>
+        <v>575.2993554822076</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -20016,7 +20016,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>575.46948768782011</v>
+        <v>575.15478686930135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20025,7 +20025,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>575.28959086369991</v>
+        <v>575.46068713664727</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -20034,7 +20034,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>575.08508739193519</v>
+        <v>575.06966230596311</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -20043,7 +20043,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>575.40921028566561</v>
+        <v>575.45710242651955</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -20052,7 +20052,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>575.22689235635187</v>
+        <v>575.05042693423331</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -20061,7 +20061,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>575.31236283415558</v>
+        <v>575.39021131716368</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -20070,7 +20070,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>575.18250676537014</v>
+        <v>575.09367627219444</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -20079,7 +20079,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>575.41130810272409</v>
+        <v>575.10028679592267</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -20088,7 +20088,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>575.18697431565647</v>
+        <v>575.40251471238901</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -20097,7 +20097,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>575.05307307466194</v>
+        <v>575.12075590197867</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -20106,7 +20106,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>575.35778045770735</v>
+        <v>575.05778053186248</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -20115,7 +20115,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>575.23185861291381</v>
+        <v>575.06356764190696</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -20124,7 +20124,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>575.11731102905867</v>
+        <v>575.26069666107969</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -20133,7 +20133,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>575.09905003538756</v>
+        <v>575.23032018929791</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -20142,7 +20142,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>575.28315352592494</v>
+        <v>575.44167479567363</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -20151,7 +20151,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>575.12919225488008</v>
+        <v>575.23379184066494</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -20160,7 +20160,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>575.02259957096885</v>
+        <v>575.18082370650973</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -20169,7 +20169,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>575.43393524493649</v>
+        <v>575.07312896096471</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -20178,7 +20178,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>575.09471214091593</v>
+        <v>575.47901307413463</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -20187,7 +20187,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>575.38573388404859</v>
+        <v>575.03166380121979</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -20196,7 +20196,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>575.36832769833552</v>
+        <v>575.45316812358669</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -20205,7 +20205,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>575.41326872018749</v>
+        <v>575.29576227331381</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -20214,7 +20214,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>575.30777440185409</v>
+        <v>575.37592946793973</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -20223,7 +20223,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>575.38109108892922</v>
+        <v>575.02856714758002</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -20232,7 +20232,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>575.48303681589675</v>
+        <v>575.36321846593535</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -20241,7 +20241,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>575.30052355909777</v>
+        <v>575.10325798546853</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -20250,7 +20250,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>575.30648825082551</v>
+        <v>575.07914831189839</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -20259,7 +20259,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>575.03391164066841</v>
+        <v>575.20032012054571</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -20268,7 +20268,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>575.11048421156318</v>
+        <v>575.29770466908565</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -20277,7 +20277,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>575.2223110811351</v>
+        <v>575.26053438738643</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -20286,7 +20286,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>575.15980490267566</v>
+        <v>575.07789613010812</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -20295,7 +20295,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>575.42273095968733</v>
+        <v>575.37043864598195</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -20304,7 +20304,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>575.36882794896553</v>
+        <v>575.22323479570923</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -20313,7 +20313,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>575.31825798669138</v>
+        <v>575.41794274802453</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -20322,7 +20322,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>575.00387707081563</v>
+        <v>575.12234939222913</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -20331,7 +20331,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>575.36570150806881</v>
+        <v>575.1498250127396</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -20340,7 +20340,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>575.33895682141303</v>
+        <v>575.05590019040812</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -20349,7 +20349,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>575.12325847454861</v>
+        <v>575.33014807214875</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -20358,7 +20358,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>575.47389699066434</v>
+        <v>575.49166380975771</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -20367,7 +20367,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>575.11422650648944</v>
+        <v>575.48608319300899</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -20376,7 +20376,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>575.00754002671044</v>
+        <v>575.0144729737417</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -20385,7 +20385,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>575.25102941803982</v>
+        <v>575.12173113940798</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -20394,7 +20394,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>575.47283372394725</v>
+        <v>575.0167043987027</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -20403,7 +20403,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>575.06946765544035</v>
+        <v>575.08099911173838</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -20412,7 +20412,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>575.27499655074837</v>
+        <v>575.25101762681743</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -20421,7 +20421,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>575.40372207320354</v>
+        <v>575.41831276814014</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -20430,7 +20430,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>575.17579901369129</v>
+        <v>575.05937006281397</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -20439,7 +20439,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>575.20998951612455</v>
+        <v>575.16422483516988</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -20448,7 +20448,7 @@
       </c>
       <c r="B53">
         <f ca="1">B52-RAND()</f>
-        <v>574.54820311023116</v>
+        <v>575.05122776961616</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -20457,7 +20457,7 @@
       </c>
       <c r="B54">
         <f t="shared" ref="B54:B113" ca="1" si="1">B53-RAND()</f>
-        <v>573.63267899932589</v>
+        <v>574.06723128206318</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -20466,7 +20466,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>572.72661322930901</v>
+        <v>573.46807604886828</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -20475,7 +20475,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>572.31407613919475</v>
+        <v>573.45481269583013</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -20484,7 +20484,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>571.36315831754564</v>
+        <v>572.85204005413618</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -20493,7 +20493,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>571.3525586030479</v>
+        <v>572.48748118693936</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -20502,7 +20502,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>570.42721571291918</v>
+        <v>571.74833556434282</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -20511,7 +20511,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>569.78508565178845</v>
+        <v>570.89153403088028</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -20520,7 +20520,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>569.48094572387822</v>
+        <v>570.54471448304048</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -20529,7 +20529,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>569.22145102062393</v>
+        <v>570.12353417955842</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -20538,7 +20538,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>568.71904748812028</v>
+        <v>570.11270668911493</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -20547,7 +20547,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>568.2625697542602</v>
+        <v>569.54856567213938</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -20556,7 +20556,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>568.052742892423</v>
+        <v>569.54200948666107</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -20565,7 +20565,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="1"/>
-        <v>567.14714522206486</v>
+        <v>568.75247474709147</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -20574,7 +20574,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="1"/>
-        <v>566.37984476971212</v>
+        <v>568.01564420366333</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -20583,7 +20583,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>566.34390030907116</v>
+        <v>567.11981551614349</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -20592,7 +20592,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>565.38213926397088</v>
+        <v>566.79173601812931</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -20601,7 +20601,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>565.136269630637</v>
+        <v>565.8653094116587</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -20610,7 +20610,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>564.25499111203465</v>
+        <v>565.15765041982729</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -20619,7 +20619,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>563.9603113044775</v>
+        <v>565.12728837900681</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -20628,7 +20628,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>563.31700230902425</v>
+        <v>564.31645641616331</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -20637,7 +20637,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>562.42629792368689</v>
+        <v>563.57594601107974</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -20646,7 +20646,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>561.83723461025636</v>
+        <v>563.43928828892263</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -20655,7 +20655,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>561.02371840759929</v>
+        <v>562.95233815697486</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -20664,7 +20664,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>560.85926015241512</v>
+        <v>562.76065093919419</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -20673,7 +20673,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="1"/>
-        <v>560.64528705701775</v>
+        <v>562.26263809505053</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -20682,7 +20682,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="1"/>
-        <v>559.82596387084197</v>
+        <v>561.97303378900938</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -20691,7 +20691,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="1"/>
-        <v>559.14182182474451</v>
+        <v>561.96676737734128</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -20700,7 +20700,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="1"/>
-        <v>559.07914975219023</v>
+        <v>561.72424563328127</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -20709,7 +20709,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="1"/>
-        <v>558.58424745920877</v>
+        <v>560.95924047516485</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -20718,7 +20718,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="1"/>
-        <v>557.95584942283051</v>
+        <v>560.5869243638067</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -20727,7 +20727,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="1"/>
-        <v>557.86247984336546</v>
+        <v>560.56685514899164</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -20736,7 +20736,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="1"/>
-        <v>557.5961045121096</v>
+        <v>559.83818792238276</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -20745,7 +20745,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="1"/>
-        <v>557.32339701311514</v>
+        <v>559.07899134799891</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -20754,7 +20754,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="1"/>
-        <v>556.84074540261622</v>
+        <v>558.45309670007987</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -20763,7 +20763,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="1"/>
-        <v>556.00808554945274</v>
+        <v>558.3229058755345</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -20772,7 +20772,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="1"/>
-        <v>555.33538078351171</v>
+        <v>557.67059182231264</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -20781,7 +20781,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="1"/>
-        <v>555.17721040559184</v>
+        <v>557.61737195684861</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -20790,7 +20790,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="1"/>
-        <v>555.16133111080785</v>
+        <v>557.24451821262073</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -20799,7 +20799,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="1"/>
-        <v>554.60897122657946</v>
+        <v>556.26372971632748</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -20808,7 +20808,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="1"/>
-        <v>554.32463198570088</v>
+        <v>555.28416981481951</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -20817,7 +20817,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="1"/>
-        <v>553.34309938624779</v>
+        <v>555.23288987969818</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -20826,7 +20826,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="1"/>
-        <v>553.16249750271299</v>
+        <v>555.16513557908536</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -20835,7 +20835,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="1"/>
-        <v>552.58585963766814</v>
+        <v>554.4499952671631</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -20844,7 +20844,7 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="1"/>
-        <v>551.87104225149153</v>
+        <v>554.36933442291331</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -20853,7 +20853,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="1"/>
-        <v>551.18993681348343</v>
+        <v>554.13371158075711</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -20862,7 +20862,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="1"/>
-        <v>550.81191995674953</v>
+        <v>553.52166282175347</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -20871,7 +20871,7 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="1"/>
-        <v>549.90703307844853</v>
+        <v>553.27438639162108</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -20880,7 +20880,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="1"/>
-        <v>549.31087535512972</v>
+        <v>553.1631137648119</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -20889,7 +20889,7 @@
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="1"/>
-        <v>548.62202036428141</v>
+        <v>553.11240517939825</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -20898,7 +20898,7 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="1"/>
-        <v>547.90738535155094</v>
+        <v>552.6201483844593</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -20907,7 +20907,7 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="1"/>
-        <v>547.74133473526274</v>
+        <v>551.63315491159449</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -20916,7 +20916,7 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="1"/>
-        <v>547.09818704735198</v>
+        <v>550.74488305169166</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -20925,7 +20925,7 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="1"/>
-        <v>546.87819198272894</v>
+        <v>550.09863449207705</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -20934,7 +20934,7 @@
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="1"/>
-        <v>546.27576589714431</v>
+        <v>549.1127832661723</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -20943,7 +20943,7 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="1"/>
-        <v>545.32080151542766</v>
+        <v>548.54587677248662</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -20952,7 +20952,7 @@
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="1"/>
-        <v>544.58553103908878</v>
+        <v>547.93336585486395</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -20961,7 +20961,7 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="1"/>
-        <v>543.89202655855911</v>
+        <v>547.74246485471485</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -20970,7 +20970,7 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="1"/>
-        <v>543.55058213250777</v>
+        <v>547.55174831636486</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -20979,7 +20979,7 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="1"/>
-        <v>543.38772203282235</v>
+        <v>547.07108523719194</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -20988,7 +20988,7 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="1"/>
-        <v>542.39413614332977</v>
+        <v>546.38112106200663</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -20997,7 +20997,7 @@
       </c>
       <c r="B114">
         <f ca="1">B113+0.1*RAND()</f>
-        <v>542.40423531431759</v>
+        <v>546.41843013690379</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -21006,7 +21006,7 @@
       </c>
       <c r="B115">
         <f t="shared" ref="B115:B178" ca="1" si="2">B114+0.1*RAND()</f>
-        <v>542.49657919465733</v>
+        <v>546.43088331265164</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -21015,7 +21015,7 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="2"/>
-        <v>542.53611736912785</v>
+        <v>546.47276481239794</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -21024,7 +21024,7 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="2"/>
-        <v>542.60676105318259</v>
+        <v>546.54711891944544</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -21033,7 +21033,7 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="2"/>
-        <v>542.61242939889132</v>
+        <v>546.62273232243274</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -21042,7 +21042,7 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="2"/>
-        <v>542.62188860644392</v>
+        <v>546.68960960511163</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -21051,7 +21051,7 @@
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="2"/>
-        <v>542.62489985473508</v>
+        <v>546.75455078739674</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -21060,7 +21060,7 @@
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="2"/>
-        <v>542.65207496081621</v>
+        <v>546.75824278694984</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -21069,7 +21069,7 @@
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="2"/>
-        <v>542.7223824542159</v>
+        <v>546.76730603229316</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -21078,7 +21078,7 @@
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="2"/>
-        <v>542.79969108355533</v>
+        <v>546.81768194767949</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -21087,7 +21087,7 @@
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="2"/>
-        <v>542.81280930225307</v>
+        <v>546.84538135694345</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -21096,7 +21096,7 @@
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="2"/>
-        <v>542.88021480119608</v>
+        <v>546.89013443508111</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -21105,7 +21105,7 @@
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="2"/>
-        <v>542.94991677477901</v>
+        <v>546.89936571610019</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -21114,7 +21114,7 @@
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="2"/>
-        <v>543.03691374070684</v>
+        <v>546.90359281575741</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -21123,7 +21123,7 @@
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="2"/>
-        <v>543.04742446001387</v>
+        <v>546.98570957997276</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -21132,7 +21132,7 @@
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="2"/>
-        <v>543.10644910794133</v>
+        <v>547.05575694937863</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -21141,7 +21141,7 @@
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="2"/>
-        <v>543.12493488268331</v>
+        <v>547.07669528822362</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -21150,7 +21150,7 @@
       </c>
       <c r="B131">
         <f t="shared" ca="1" si="2"/>
-        <v>543.12627892354772</v>
+        <v>547.10691630264944</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -21159,7 +21159,7 @@
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="2"/>
-        <v>543.19504009610239</v>
+        <v>547.19164969160602</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -21168,7 +21168,7 @@
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="2"/>
-        <v>543.23125192591874</v>
+        <v>547.24155357158963</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -21177,7 +21177,7 @@
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="2"/>
-        <v>543.30832062322429</v>
+        <v>547.24205621372835</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -21186,7 +21186,7 @@
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="2"/>
-        <v>543.34626441539729</v>
+        <v>547.28364842057101</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -21195,7 +21195,7 @@
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="2"/>
-        <v>543.41706642322151</v>
+        <v>547.29736115861874</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -21204,7 +21204,7 @@
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="2"/>
-        <v>543.50830594206673</v>
+        <v>547.3243617887523</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -21213,7 +21213,7 @@
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="2"/>
-        <v>543.52536213041628</v>
+        <v>547.39008521048868</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -21222,7 +21222,7 @@
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="2"/>
-        <v>543.5587276181426</v>
+        <v>547.47033087175112</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -21231,7 +21231,7 @@
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="2"/>
-        <v>543.61995141485204</v>
+        <v>547.51802110417555</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -21240,7 +21240,7 @@
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="2"/>
-        <v>543.65164066604052</v>
+        <v>547.53358051780867</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -21249,7 +21249,7 @@
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="2"/>
-        <v>543.6673228825772</v>
+        <v>547.5361920893489</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -21258,7 +21258,7 @@
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="2"/>
-        <v>543.69978235844951</v>
+        <v>547.55727927912403</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -21267,7 +21267,7 @@
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="2"/>
-        <v>543.77283092256869</v>
+        <v>547.573803373038</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -21276,7 +21276,7 @@
       </c>
       <c r="B145">
         <f t="shared" ca="1" si="2"/>
-        <v>543.80060263792063</v>
+        <v>547.62377641764658</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -21285,7 +21285,7 @@
       </c>
       <c r="B146">
         <f t="shared" ca="1" si="2"/>
-        <v>543.82117005713292</v>
+        <v>547.63058217127104</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -21294,7 +21294,7 @@
       </c>
       <c r="B147">
         <f t="shared" ca="1" si="2"/>
-        <v>543.84315775198468</v>
+        <v>547.6410344554522</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -21303,7 +21303,7 @@
       </c>
       <c r="B148">
         <f t="shared" ca="1" si="2"/>
-        <v>543.93676438442662</v>
+        <v>547.69048734705359</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -21312,7 +21312,7 @@
       </c>
       <c r="B149">
         <f t="shared" ca="1" si="2"/>
-        <v>543.97350912958154</v>
+        <v>547.71549734159419</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -21321,7 +21321,7 @@
       </c>
       <c r="B150">
         <f t="shared" ca="1" si="2"/>
-        <v>543.98125534567828</v>
+        <v>547.73179302257188</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -21330,7 +21330,7 @@
       </c>
       <c r="B151">
         <f t="shared" ca="1" si="2"/>
-        <v>544.07935105639194</v>
+        <v>547.77550500055099</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -21339,7 +21339,7 @@
       </c>
       <c r="B152">
         <f t="shared" ca="1" si="2"/>
-        <v>544.15824726054302</v>
+        <v>547.82809539682069</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -21348,7 +21348,7 @@
       </c>
       <c r="B153">
         <f t="shared" ca="1" si="2"/>
-        <v>544.25693132841877</v>
+        <v>547.85876081118101</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -21357,7 +21357,7 @@
       </c>
       <c r="B154">
         <f t="shared" ca="1" si="2"/>
-        <v>544.27389045614575</v>
+        <v>547.87256501789409</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -21366,7 +21366,7 @@
       </c>
       <c r="B155">
         <f t="shared" ca="1" si="2"/>
-        <v>544.34210481596688</v>
+        <v>547.87703589085061</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -21375,7 +21375,7 @@
       </c>
       <c r="B156">
         <f t="shared" ca="1" si="2"/>
-        <v>544.43042406614336</v>
+        <v>547.90348290411612</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -21384,7 +21384,7 @@
       </c>
       <c r="B157">
         <f t="shared" ca="1" si="2"/>
-        <v>544.49537057754526</v>
+        <v>547.94772201160447</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -21393,7 +21393,7 @@
       </c>
       <c r="B158">
         <f t="shared" ca="1" si="2"/>
-        <v>544.54867153504381</v>
+        <v>547.96553622400245</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -21402,7 +21402,7 @@
       </c>
       <c r="B159">
         <f t="shared" ca="1" si="2"/>
-        <v>544.64236666752606</v>
+        <v>548.02171710426876</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -21411,7 +21411,7 @@
       </c>
       <c r="B160">
         <f t="shared" ca="1" si="2"/>
-        <v>544.66583176199458</v>
+        <v>548.07688571137055</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -21420,7 +21420,7 @@
       </c>
       <c r="B161">
         <f t="shared" ca="1" si="2"/>
-        <v>544.67718560573405</v>
+        <v>548.10938276464515</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -21429,7 +21429,7 @@
       </c>
       <c r="B162">
         <f t="shared" ca="1" si="2"/>
-        <v>544.7501505167171</v>
+        <v>548.17313807361461</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -21438,7 +21438,7 @@
       </c>
       <c r="B163">
         <f t="shared" ca="1" si="2"/>
-        <v>544.80918817244583</v>
+        <v>548.21174465030197</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -21447,7 +21447,7 @@
       </c>
       <c r="B164">
         <f t="shared" ca="1" si="2"/>
-        <v>544.88161933977779</v>
+        <v>548.23437311727412</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -21456,7 +21456,7 @@
       </c>
       <c r="B165">
         <f t="shared" ca="1" si="2"/>
-        <v>544.93054357464246</v>
+        <v>548.28787288608771</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -21465,7 +21465,7 @@
       </c>
       <c r="B166">
         <f t="shared" ca="1" si="2"/>
-        <v>544.93622568945932</v>
+        <v>548.37264396108151</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -21474,7 +21474,7 @@
       </c>
       <c r="B167">
         <f t="shared" ca="1" si="2"/>
-        <v>545.03306493857224</v>
+        <v>548.3796646690563</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -21483,7 +21483,7 @@
       </c>
       <c r="B168">
         <f t="shared" ca="1" si="2"/>
-        <v>545.08228564078763</v>
+        <v>548.42871268086515</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -21492,7 +21492,7 @@
       </c>
       <c r="B169">
         <f t="shared" ca="1" si="2"/>
-        <v>545.1511258973328</v>
+        <v>548.50862079090791</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -21501,7 +21501,7 @@
       </c>
       <c r="B170">
         <f t="shared" ca="1" si="2"/>
-        <v>545.18249683385841</v>
+        <v>548.53177026348874</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -21510,7 +21510,7 @@
       </c>
       <c r="B171">
         <f t="shared" ca="1" si="2"/>
-        <v>545.20749829097895</v>
+        <v>548.61030931776088</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -21519,7 +21519,7 @@
       </c>
       <c r="B172">
         <f t="shared" ca="1" si="2"/>
-        <v>545.29871527440787</v>
+        <v>548.61830165915592</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -21528,7 +21528,7 @@
       </c>
       <c r="B173">
         <f t="shared" ca="1" si="2"/>
-        <v>545.32314985067603</v>
+        <v>548.70368129998735</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -21537,7 +21537,7 @@
       </c>
       <c r="B174">
         <f t="shared" ca="1" si="2"/>
-        <v>545.32484619715194</v>
+        <v>548.7222495264524</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -21546,7 +21546,7 @@
       </c>
       <c r="B175">
         <f t="shared" ca="1" si="2"/>
-        <v>545.36941505098753</v>
+        <v>548.7831990824385</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -21555,7 +21555,7 @@
       </c>
       <c r="B176">
         <f t="shared" ca="1" si="2"/>
-        <v>545.41328182254949</v>
+        <v>548.84401017831487</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -21564,7 +21564,7 @@
       </c>
       <c r="B177">
         <f t="shared" ca="1" si="2"/>
-        <v>545.46114854938628</v>
+        <v>548.92764075088803</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -21573,7 +21573,7 @@
       </c>
       <c r="B178">
         <f t="shared" ca="1" si="2"/>
-        <v>545.51655159098527</v>
+        <v>549.00073043676946</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -21582,7 +21582,7 @@
       </c>
       <c r="B179">
         <f t="shared" ref="B179:B242" ca="1" si="3">B178+0.1*RAND()</f>
-        <v>545.5775532562194</v>
+        <v>549.03629741147472</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -21591,7 +21591,7 @@
       </c>
       <c r="B180">
         <f t="shared" ca="1" si="3"/>
-        <v>545.64010559936833</v>
+        <v>549.05774709436321</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -21600,7 +21600,7 @@
       </c>
       <c r="B181">
         <f t="shared" ca="1" si="3"/>
-        <v>545.708598592474</v>
+        <v>549.08482794699853</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -21609,7 +21609,7 @@
       </c>
       <c r="B182">
         <f t="shared" ca="1" si="3"/>
-        <v>545.79988573636126</v>
+        <v>549.09921249740887</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -21618,7 +21618,7 @@
       </c>
       <c r="B183">
         <f t="shared" ca="1" si="3"/>
-        <v>545.80431780682341</v>
+        <v>549.19189257588573</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -21627,7 +21627,7 @@
       </c>
       <c r="B184">
         <f t="shared" ca="1" si="3"/>
-        <v>545.85877788236473</v>
+        <v>549.2840439554426</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -21636,7 +21636,7 @@
       </c>
       <c r="B185">
         <f t="shared" ca="1" si="3"/>
-        <v>545.87791619112397</v>
+        <v>549.28748140594996</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -21645,7 +21645,7 @@
       </c>
       <c r="B186">
         <f t="shared" ca="1" si="3"/>
-        <v>545.93902195810097</v>
+        <v>549.36250790105817</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -21654,7 +21654,7 @@
       </c>
       <c r="B187">
         <f t="shared" ca="1" si="3"/>
-        <v>546.02871379874193</v>
+        <v>549.39501794296075</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -21663,7 +21663,7 @@
       </c>
       <c r="B188">
         <f t="shared" ca="1" si="3"/>
-        <v>546.0713129459657</v>
+        <v>549.44507081444192</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -21672,7 +21672,7 @@
       </c>
       <c r="B189">
         <f t="shared" ca="1" si="3"/>
-        <v>546.16033196847809</v>
+        <v>549.46707071963385</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -21681,7 +21681,7 @@
       </c>
       <c r="B190">
         <f t="shared" ca="1" si="3"/>
-        <v>546.24061337745673</v>
+        <v>549.5637697011739</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -21690,7 +21690,7 @@
       </c>
       <c r="B191">
         <f t="shared" ca="1" si="3"/>
-        <v>546.25672007690503</v>
+        <v>549.63437475130866</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -21699,7 +21699,7 @@
       </c>
       <c r="B192">
         <f t="shared" ca="1" si="3"/>
-        <v>546.32320957168884</v>
+        <v>549.65828291980517</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -21708,7 +21708,7 @@
       </c>
       <c r="B193">
         <f t="shared" ca="1" si="3"/>
-        <v>546.33242395436719</v>
+        <v>549.66983833379675</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -21717,7 +21717,7 @@
       </c>
       <c r="B194">
         <f t="shared" ca="1" si="3"/>
-        <v>546.33779036531723</v>
+        <v>549.75429136712614</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -21726,7 +21726,7 @@
       </c>
       <c r="B195">
         <f t="shared" ca="1" si="3"/>
-        <v>546.43479156001854</v>
+        <v>549.80323921066406</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -21735,7 +21735,7 @@
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="3"/>
-        <v>546.45040772300058</v>
+        <v>549.88663309090771</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -21744,7 +21744,7 @@
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="3"/>
-        <v>546.50385546954067</v>
+        <v>549.92860553877756</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -21753,7 +21753,7 @@
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="3"/>
-        <v>546.54788947155498</v>
+        <v>549.96790589688976</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -21762,7 +21762,7 @@
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="3"/>
-        <v>546.63054968405106</v>
+        <v>549.99278467936506</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -21771,7 +21771,7 @@
       </c>
       <c r="B200">
         <f t="shared" ca="1" si="3"/>
-        <v>546.69603944907681</v>
+        <v>550.08818694373122</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -21780,7 +21780,7 @@
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="3"/>
-        <v>546.78258861196946</v>
+        <v>550.09200262927209</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -21789,7 +21789,7 @@
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="3"/>
-        <v>546.86781775681288</v>
+        <v>550.12268523996784</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -21798,7 +21798,7 @@
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="3"/>
-        <v>546.95672408638575</v>
+        <v>550.1628469686126</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -21807,7 +21807,7 @@
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="3"/>
-        <v>546.98180931675176</v>
+        <v>550.24791183820105</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -21816,7 +21816,7 @@
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="3"/>
-        <v>547.04249541609954</v>
+        <v>550.28304832440801</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -21825,7 +21825,7 @@
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="3"/>
-        <v>547.1077292962982</v>
+        <v>550.31153269125218</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -21834,7 +21834,7 @@
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="3"/>
-        <v>547.11804963656607</v>
+        <v>550.37785994532476</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -21843,7 +21843,7 @@
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="3"/>
-        <v>547.16201437058908</v>
+        <v>550.38041057345777</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -21852,7 +21852,7 @@
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="3"/>
-        <v>547.24489040570427</v>
+        <v>550.46373888834489</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -21861,7 +21861,7 @@
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="3"/>
-        <v>547.26570836945029</v>
+        <v>550.53689019265948</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -21870,7 +21870,7 @@
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="3"/>
-        <v>547.27105839935564</v>
+        <v>550.58513575086045</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -21879,7 +21879,7 @@
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="3"/>
-        <v>547.3572653799223</v>
+        <v>550.5895102196497</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -21888,7 +21888,7 @@
       </c>
       <c r="B213">
         <f t="shared" ca="1" si="3"/>
-        <v>547.40260582043152</v>
+        <v>550.59547685834821</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -21897,7 +21897,7 @@
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="3"/>
-        <v>547.43807912928025</v>
+        <v>550.62356415641091</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -21906,7 +21906,7 @@
       </c>
       <c r="B215">
         <f t="shared" ca="1" si="3"/>
-        <v>547.47358581575395</v>
+        <v>550.67055967670547</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -21915,7 +21915,7 @@
       </c>
       <c r="B216">
         <f t="shared" ca="1" si="3"/>
-        <v>547.50317266740126</v>
+        <v>550.73780466888718</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -21924,7 +21924,7 @@
       </c>
       <c r="B217">
         <f t="shared" ca="1" si="3"/>
-        <v>547.55920634372251</v>
+        <v>550.81643354092137</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -21933,7 +21933,7 @@
       </c>
       <c r="B218">
         <f t="shared" ca="1" si="3"/>
-        <v>547.63674155725857</v>
+        <v>550.90685375572366</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -21942,7 +21942,7 @@
       </c>
       <c r="B219">
         <f t="shared" ca="1" si="3"/>
-        <v>547.66310226757435</v>
+        <v>550.91853936293262</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -21951,7 +21951,7 @@
       </c>
       <c r="B220">
         <f t="shared" ca="1" si="3"/>
-        <v>547.72924707869367</v>
+        <v>551.01608606860702</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -21960,7 +21960,7 @@
       </c>
       <c r="B221">
         <f t="shared" ca="1" si="3"/>
-        <v>547.80645954676993</v>
+        <v>551.02204149544548</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -21969,7 +21969,7 @@
       </c>
       <c r="B222">
         <f t="shared" ca="1" si="3"/>
-        <v>547.86784722037999</v>
+        <v>551.11456970122686</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -21978,7 +21978,7 @@
       </c>
       <c r="B223">
         <f t="shared" ca="1" si="3"/>
-        <v>547.91646105535392</v>
+        <v>551.15254765866769</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -21987,7 +21987,7 @@
       </c>
       <c r="B224">
         <f t="shared" ca="1" si="3"/>
-        <v>547.91808448904112</v>
+        <v>551.20242302331997</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -21996,7 +21996,7 @@
       </c>
       <c r="B225">
         <f t="shared" ca="1" si="3"/>
-        <v>547.94795675908892</v>
+        <v>551.20866423024484</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -22005,7 +22005,7 @@
       </c>
       <c r="B226">
         <f t="shared" ca="1" si="3"/>
-        <v>547.99855711441603</v>
+        <v>551.30848769770625</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -22014,7 +22014,7 @@
       </c>
       <c r="B227">
         <f t="shared" ca="1" si="3"/>
-        <v>548.05730112381343</v>
+        <v>551.4060130989177</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -22023,7 +22023,7 @@
       </c>
       <c r="B228">
         <f t="shared" ca="1" si="3"/>
-        <v>548.11764929905542</v>
+        <v>551.49364221379017</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -22032,7 +22032,7 @@
       </c>
       <c r="B229">
         <f t="shared" ca="1" si="3"/>
-        <v>548.1422198094433</v>
+        <v>551.57309278851449</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -22041,7 +22041,7 @@
       </c>
       <c r="B230">
         <f t="shared" ca="1" si="3"/>
-        <v>548.23037475047272</v>
+        <v>551.63764852335089</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -22050,7 +22050,7 @@
       </c>
       <c r="B231">
         <f t="shared" ca="1" si="3"/>
-        <v>548.23304843498215</v>
+        <v>551.64341084794421</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -22059,7 +22059,7 @@
       </c>
       <c r="B232">
         <f t="shared" ca="1" si="3"/>
-        <v>548.28258005846089</v>
+        <v>551.68525988724764</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -22068,7 +22068,7 @@
       </c>
       <c r="B233">
         <f t="shared" ca="1" si="3"/>
-        <v>548.3269687157117</v>
+        <v>551.70825904488504</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -22077,7 +22077,7 @@
       </c>
       <c r="B234">
         <f t="shared" ca="1" si="3"/>
-        <v>548.41833644836095</v>
+        <v>551.73361582889413</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -22086,7 +22086,7 @@
       </c>
       <c r="B235">
         <f t="shared" ca="1" si="3"/>
-        <v>548.51661118292657</v>
+        <v>551.79414100101394</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -22095,7 +22095,7 @@
       </c>
       <c r="B236">
         <f t="shared" ca="1" si="3"/>
-        <v>548.54024219797395</v>
+        <v>551.80391583730488</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -22104,7 +22104,7 @@
       </c>
       <c r="B237">
         <f t="shared" ca="1" si="3"/>
-        <v>548.54518001163103</v>
+        <v>551.88151632757683</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -22113,7 +22113,7 @@
       </c>
       <c r="B238">
         <f t="shared" ca="1" si="3"/>
-        <v>548.63650690191184</v>
+        <v>551.91545832680799</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -22122,7 +22122,7 @@
       </c>
       <c r="B239">
         <f t="shared" ca="1" si="3"/>
-        <v>548.69936969537832</v>
+        <v>551.96868744539688</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -22131,7 +22131,7 @@
       </c>
       <c r="B240">
         <f t="shared" ca="1" si="3"/>
-        <v>548.71371293743425</v>
+        <v>552.01964492778598</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -22140,7 +22140,7 @@
       </c>
       <c r="B241">
         <f t="shared" ca="1" si="3"/>
-        <v>548.73056428245388</v>
+        <v>552.04032903220013</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -22149,7 +22149,7 @@
       </c>
       <c r="B242">
         <f t="shared" ca="1" si="3"/>
-        <v>548.80292770984238</v>
+        <v>552.10807087496266</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -22158,7 +22158,7 @@
       </c>
       <c r="B243">
         <f t="shared" ref="B243:B306" ca="1" si="4">B242+0.1*RAND()</f>
-        <v>548.89704702512063</v>
+        <v>552.11038496560411</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -22167,7 +22167,7 @@
       </c>
       <c r="B244">
         <f t="shared" ca="1" si="4"/>
-        <v>548.95478858713557</v>
+        <v>552.18828203427461</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -22176,7 +22176,7 @@
       </c>
       <c r="B245">
         <f t="shared" ca="1" si="4"/>
-        <v>548.98370709568826</v>
+        <v>552.26045377752428</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -22185,7 +22185,7 @@
       </c>
       <c r="B246">
         <f t="shared" ca="1" si="4"/>
-        <v>549.00881834601353</v>
+        <v>552.31832822776403</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -22194,7 +22194,7 @@
       </c>
       <c r="B247">
         <f t="shared" ca="1" si="4"/>
-        <v>549.05355102138594</v>
+        <v>552.39471115868514</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -22203,7 +22203,7 @@
       </c>
       <c r="B248">
         <f t="shared" ca="1" si="4"/>
-        <v>549.1375363339929</v>
+        <v>552.45707107196006</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -22212,7 +22212,7 @@
       </c>
       <c r="B249">
         <f t="shared" ca="1" si="4"/>
-        <v>549.18392737055888</v>
+        <v>552.54110356117008</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -22221,7 +22221,7 @@
       </c>
       <c r="B250">
         <f t="shared" ca="1" si="4"/>
-        <v>549.27076509482436</v>
+        <v>552.63023866440494</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -22230,7 +22230,7 @@
       </c>
       <c r="B251">
         <f t="shared" ca="1" si="4"/>
-        <v>549.30409238094148</v>
+        <v>552.66482293002025</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -22239,7 +22239,7 @@
       </c>
       <c r="B252">
         <f t="shared" ca="1" si="4"/>
-        <v>549.32946898745308</v>
+        <v>552.74223313628067</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -22248,7 +22248,7 @@
       </c>
       <c r="B253">
         <f t="shared" ca="1" si="4"/>
-        <v>549.38034121000021</v>
+        <v>552.7666234128784</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -22257,7 +22257,7 @@
       </c>
       <c r="B254">
         <f t="shared" ca="1" si="4"/>
-        <v>549.40299960583468</v>
+        <v>552.8195753491691</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -22266,7 +22266,7 @@
       </c>
       <c r="B255">
         <f t="shared" ca="1" si="4"/>
-        <v>549.45336473117925</v>
+        <v>552.83656545478379</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -22275,7 +22275,7 @@
       </c>
       <c r="B256">
         <f t="shared" ca="1" si="4"/>
-        <v>549.52405106317667</v>
+        <v>552.93384618041091</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -22284,7 +22284,7 @@
       </c>
       <c r="B257">
         <f t="shared" ca="1" si="4"/>
-        <v>549.54767130036032</v>
+        <v>552.94864233092608</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -22293,7 +22293,7 @@
       </c>
       <c r="B258">
         <f t="shared" ca="1" si="4"/>
-        <v>549.55454783570917</v>
+        <v>553.04065279447764</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -22302,7 +22302,7 @@
       </c>
       <c r="B259">
         <f t="shared" ca="1" si="4"/>
-        <v>549.64679784121324</v>
+        <v>553.08786120366494</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -22311,7 +22311,7 @@
       </c>
       <c r="B260">
         <f t="shared" ca="1" si="4"/>
-        <v>549.70631988099012</v>
+        <v>553.15329999570599</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -22320,7 +22320,7 @@
       </c>
       <c r="B261">
         <f t="shared" ca="1" si="4"/>
-        <v>549.73942500743465</v>
+        <v>553.16844184182207</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -22329,7 +22329,7 @@
       </c>
       <c r="B262">
         <f t="shared" ca="1" si="4"/>
-        <v>549.82284287621826</v>
+        <v>553.23404583023478</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
@@ -22338,7 +22338,7 @@
       </c>
       <c r="B263">
         <f t="shared" ca="1" si="4"/>
-        <v>549.88615611008413</v>
+        <v>553.265946398246</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -22347,7 +22347,7 @@
       </c>
       <c r="B264">
         <f t="shared" ca="1" si="4"/>
-        <v>549.93273870543749</v>
+        <v>553.35172617515627</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -22356,7 +22356,7 @@
       </c>
       <c r="B265">
         <f t="shared" ca="1" si="4"/>
-        <v>549.98762380418771</v>
+        <v>553.44493517732406</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -22365,7 +22365,7 @@
       </c>
       <c r="B266">
         <f t="shared" ca="1" si="4"/>
-        <v>550.0180223678417</v>
+        <v>553.52853418235679</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
@@ -22374,7 +22374,7 @@
       </c>
       <c r="B267">
         <f t="shared" ca="1" si="4"/>
-        <v>550.11078780276807</v>
+        <v>553.55355963606496</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -22383,7 +22383,7 @@
       </c>
       <c r="B268">
         <f t="shared" ca="1" si="4"/>
-        <v>550.20366755511441</v>
+        <v>553.56336998360609</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
@@ -22392,7 +22392,7 @@
       </c>
       <c r="B269">
         <f t="shared" ca="1" si="4"/>
-        <v>550.26471274934772</v>
+        <v>553.59416656110818</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
@@ -22401,7 +22401,7 @@
       </c>
       <c r="B270">
         <f t="shared" ca="1" si="4"/>
-        <v>550.33882471147444</v>
+        <v>553.6018810842445</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -22410,7 +22410,7 @@
       </c>
       <c r="B271">
         <f t="shared" ca="1" si="4"/>
-        <v>550.40297455068662</v>
+        <v>553.64904185983585</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
@@ -22419,7 +22419,7 @@
       </c>
       <c r="B272">
         <f t="shared" ca="1" si="4"/>
-        <v>550.46170502145071</v>
+        <v>553.66320803011661</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
@@ -22428,7 +22428,7 @@
       </c>
       <c r="B273">
         <f t="shared" ca="1" si="4"/>
-        <v>550.52224847417699</v>
+        <v>553.68667413615219</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -22437,7 +22437,7 @@
       </c>
       <c r="B274">
         <f t="shared" ca="1" si="4"/>
-        <v>550.58621497237414</v>
+        <v>553.75155074201064</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -22446,7 +22446,7 @@
       </c>
       <c r="B275">
         <f t="shared" ca="1" si="4"/>
-        <v>550.62142877876715</v>
+        <v>553.8258154010756</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -22455,7 +22455,7 @@
       </c>
       <c r="B276">
         <f t="shared" ca="1" si="4"/>
-        <v>550.64523775828422</v>
+        <v>553.87459630703154</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -22464,7 +22464,7 @@
       </c>
       <c r="B277">
         <f t="shared" ca="1" si="4"/>
-        <v>550.67864228352823</v>
+        <v>553.9567403578335</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -22473,7 +22473,7 @@
       </c>
       <c r="B278">
         <f t="shared" ca="1" si="4"/>
-        <v>550.76234906957154</v>
+        <v>554.04102520660945</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
@@ -22482,7 +22482,7 @@
       </c>
       <c r="B279">
         <f t="shared" ca="1" si="4"/>
-        <v>550.84039581109528</v>
+        <v>554.11685182984309</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -22491,7 +22491,7 @@
       </c>
       <c r="B280">
         <f t="shared" ca="1" si="4"/>
-        <v>550.86446739730729</v>
+        <v>554.15957085679986</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
@@ -22500,7 +22500,7 @@
       </c>
       <c r="B281">
         <f t="shared" ca="1" si="4"/>
-        <v>550.95653132327357</v>
+        <v>554.23672391161892</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
@@ -22509,7 +22509,7 @@
       </c>
       <c r="B282">
         <f t="shared" ca="1" si="4"/>
-        <v>551.03284425955167</v>
+        <v>554.25910506820571</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -22518,7 +22518,7 @@
       </c>
       <c r="B283">
         <f t="shared" ca="1" si="4"/>
-        <v>551.08365662271888</v>
+        <v>554.34182137042194</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
@@ -22527,7 +22527,7 @@
       </c>
       <c r="B284">
         <f t="shared" ca="1" si="4"/>
-        <v>551.14541168635333</v>
+        <v>554.42367591725952</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -22536,7 +22536,7 @@
       </c>
       <c r="B285">
         <f t="shared" ca="1" si="4"/>
-        <v>551.1726496999579</v>
+        <v>554.50720699504291</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -22545,7 +22545,7 @@
       </c>
       <c r="B286">
         <f t="shared" ca="1" si="4"/>
-        <v>551.25257174301771</v>
+        <v>554.53550618035615</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
@@ -22554,7 +22554,7 @@
       </c>
       <c r="B287">
         <f t="shared" ca="1" si="4"/>
-        <v>551.25384101514601</v>
+        <v>554.54495320103536</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
@@ -22563,7 +22563,7 @@
       </c>
       <c r="B288">
         <f t="shared" ca="1" si="4"/>
-        <v>551.32640106887925</v>
+        <v>554.62247044515061</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -22572,7 +22572,7 @@
       </c>
       <c r="B289">
         <f t="shared" ca="1" si="4"/>
-        <v>551.40823469419161</v>
+        <v>554.69528569289639</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
@@ -22581,7 +22581,7 @@
       </c>
       <c r="B290">
         <f t="shared" ca="1" si="4"/>
-        <v>551.4936553520555</v>
+        <v>554.74546926440769</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
@@ -22590,7 +22590,7 @@
       </c>
       <c r="B291">
         <f t="shared" ca="1" si="4"/>
-        <v>551.54473771543962</v>
+        <v>554.82679049028616</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -22599,7 +22599,7 @@
       </c>
       <c r="B292">
         <f t="shared" ca="1" si="4"/>
-        <v>551.58430243662053</v>
+        <v>554.88617944625969</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
@@ -22608,7 +22608,7 @@
       </c>
       <c r="B293">
         <f t="shared" ca="1" si="4"/>
-        <v>551.58695849617607</v>
+        <v>554.95270045462678</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
@@ -22617,7 +22617,7 @@
       </c>
       <c r="B294">
         <f t="shared" ca="1" si="4"/>
-        <v>551.58905234704014</v>
+        <v>554.98127368464543</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -22626,7 +22626,7 @@
       </c>
       <c r="B295">
         <f t="shared" ca="1" si="4"/>
-        <v>551.60054750168661</v>
+        <v>555.00393356208713</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
@@ -22635,7 +22635,7 @@
       </c>
       <c r="B296">
         <f t="shared" ca="1" si="4"/>
-        <v>551.60569993994318</v>
+        <v>555.05933069221612</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -22644,7 +22644,7 @@
       </c>
       <c r="B297">
         <f t="shared" ca="1" si="4"/>
-        <v>551.66515256559387</v>
+        <v>555.14770521250603</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -22653,7 +22653,7 @@
       </c>
       <c r="B298">
         <f t="shared" ca="1" si="4"/>
-        <v>551.75595701864643</v>
+        <v>555.18831595960546</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -22662,7 +22662,7 @@
       </c>
       <c r="B299">
         <f t="shared" ca="1" si="4"/>
-        <v>551.84362217575381</v>
+        <v>555.22849286275721</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -22671,7 +22671,7 @@
       </c>
       <c r="B300">
         <f t="shared" ca="1" si="4"/>
-        <v>551.87474783372897</v>
+        <v>555.24097494296961</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -22680,7 +22680,7 @@
       </c>
       <c r="B301">
         <f t="shared" ca="1" si="4"/>
-        <v>551.87995014784201</v>
+        <v>555.25785473945359</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -22689,7 +22689,7 @@
       </c>
       <c r="B302">
         <f t="shared" ca="1" si="4"/>
-        <v>551.91195019394945</v>
+        <v>555.34995352426097</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -22698,7 +22698,7 @@
       </c>
       <c r="B303">
         <f t="shared" ca="1" si="4"/>
-        <v>551.92594662515114</v>
+        <v>555.44063120169983</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -22707,7 +22707,7 @@
       </c>
       <c r="B304">
         <f t="shared" ca="1" si="4"/>
-        <v>552.0252614813902</v>
+        <v>555.44313258889031</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -22716,7 +22716,7 @@
       </c>
       <c r="B305">
         <f t="shared" ca="1" si="4"/>
-        <v>552.09555240880616</v>
+        <v>555.52230717494479</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -22725,7 +22725,7 @@
       </c>
       <c r="B306">
         <f t="shared" ca="1" si="4"/>
-        <v>552.13801729075635</v>
+        <v>555.57452883253825</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -22734,7 +22734,7 @@
       </c>
       <c r="B307">
         <f t="shared" ref="B307:B370" ca="1" si="5">B306+0.1*RAND()</f>
-        <v>552.14159163803004</v>
+        <v>555.64510430645805</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -22743,7 +22743,7 @@
       </c>
       <c r="B308">
         <f t="shared" ca="1" si="5"/>
-        <v>552.17401328094786</v>
+        <v>555.6525319194858</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
@@ -22752,7 +22752,7 @@
       </c>
       <c r="B309">
         <f t="shared" ca="1" si="5"/>
-        <v>552.18600994732628</v>
+        <v>555.72619715737494</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -22761,7 +22761,7 @@
       </c>
       <c r="B310">
         <f t="shared" ca="1" si="5"/>
-        <v>552.26728032569565</v>
+        <v>555.74909077612358</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
@@ -22770,7 +22770,7 @@
       </c>
       <c r="B311">
         <f t="shared" ca="1" si="5"/>
-        <v>552.32066000836778</v>
+        <v>555.82223517436773</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -22779,7 +22779,7 @@
       </c>
       <c r="B312">
         <f t="shared" ca="1" si="5"/>
-        <v>552.41490818675982</v>
+        <v>555.8306055527878</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -22788,7 +22788,7 @@
       </c>
       <c r="B313">
         <f t="shared" ca="1" si="5"/>
-        <v>552.48120764713758</v>
+        <v>555.90551647535483</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
@@ -22797,7 +22797,7 @@
       </c>
       <c r="B314">
         <f t="shared" ca="1" si="5"/>
-        <v>552.49895961229288</v>
+        <v>555.96434699170823</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
@@ -22806,7 +22806,7 @@
       </c>
       <c r="B315">
         <f t="shared" ca="1" si="5"/>
-        <v>552.53448529980028</v>
+        <v>556.05077643346158</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -22815,7 +22815,7 @@
       </c>
       <c r="B316">
         <f t="shared" ca="1" si="5"/>
-        <v>552.58386127524091</v>
+        <v>556.1249315636212</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
@@ -22824,7 +22824,7 @@
       </c>
       <c r="B317">
         <f t="shared" ca="1" si="5"/>
-        <v>552.61677630084819</v>
+        <v>556.16257192981118</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
@@ -22833,7 +22833,7 @@
       </c>
       <c r="B318">
         <f t="shared" ca="1" si="5"/>
-        <v>552.64559523877438</v>
+        <v>556.24761406422635</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -22842,7 +22842,7 @@
       </c>
       <c r="B319">
         <f t="shared" ca="1" si="5"/>
-        <v>552.70253371828653</v>
+        <v>556.26383410399808</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
@@ -22851,7 +22851,7 @@
       </c>
       <c r="B320">
         <f t="shared" ca="1" si="5"/>
-        <v>552.73203068996384</v>
+        <v>556.27253875887743</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -22860,7 +22860,7 @@
       </c>
       <c r="B321">
         <f t="shared" ca="1" si="5"/>
-        <v>552.73726468869575</v>
+        <v>556.33952250481752</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -22869,7 +22869,7 @@
       </c>
       <c r="B322">
         <f t="shared" ca="1" si="5"/>
-        <v>552.76148342843157</v>
+        <v>556.41754756305659</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -22878,7 +22878,7 @@
       </c>
       <c r="B323">
         <f t="shared" ca="1" si="5"/>
-        <v>552.82227187432829</v>
+        <v>556.46032400297292</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -22887,7 +22887,7 @@
       </c>
       <c r="B324">
         <f t="shared" ca="1" si="5"/>
-        <v>552.86755618003156</v>
+        <v>556.49635274201682</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -22896,7 +22896,7 @@
       </c>
       <c r="B325">
         <f t="shared" ca="1" si="5"/>
-        <v>552.93084550910953</v>
+        <v>556.53306435255274</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
@@ -22905,7 +22905,7 @@
       </c>
       <c r="B326">
         <f t="shared" ca="1" si="5"/>
-        <v>553.0119263177952</v>
+        <v>556.61564954013147</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
@@ -22914,7 +22914,7 @@
       </c>
       <c r="B327">
         <f t="shared" ca="1" si="5"/>
-        <v>553.09708062138873</v>
+        <v>556.68364139336666</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -22923,7 +22923,7 @@
       </c>
       <c r="B328">
         <f t="shared" ca="1" si="5"/>
-        <v>553.15752512268909</v>
+        <v>556.77570091961297</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
@@ -22932,7 +22932,7 @@
       </c>
       <c r="B329">
         <f t="shared" ca="1" si="5"/>
-        <v>553.21507146683314</v>
+        <v>556.79362651636131</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -22941,7 +22941,7 @@
       </c>
       <c r="B330">
         <f t="shared" ca="1" si="5"/>
-        <v>553.29740106970644</v>
+        <v>556.79781339952945</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -22950,7 +22950,7 @@
       </c>
       <c r="B331">
         <f t="shared" ca="1" si="5"/>
-        <v>553.34261673302228</v>
+        <v>556.88226640430389</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -22959,7 +22959,7 @@
       </c>
       <c r="B332">
         <f t="shared" ca="1" si="5"/>
-        <v>553.42435158904061</v>
+        <v>556.88957523768556</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -22968,7 +22968,7 @@
       </c>
       <c r="B333">
         <f t="shared" ca="1" si="5"/>
-        <v>553.51575729180547</v>
+        <v>556.89384717691109</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -22977,7 +22977,7 @@
       </c>
       <c r="B334">
         <f t="shared" ca="1" si="5"/>
-        <v>553.54691157544346</v>
+        <v>556.94013809777368</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
@@ -22986,7 +22986,7 @@
       </c>
       <c r="B335">
         <f t="shared" ca="1" si="5"/>
-        <v>553.62446731713624</v>
+        <v>557.00137617919881</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
@@ -22995,7 +22995,7 @@
       </c>
       <c r="B336">
         <f t="shared" ca="1" si="5"/>
-        <v>553.64235937935609</v>
+        <v>557.10017449038719</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -23004,7 +23004,7 @@
       </c>
       <c r="B337">
         <f t="shared" ca="1" si="5"/>
-        <v>553.6556225826339</v>
+        <v>557.17647735531386</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
@@ -23013,7 +23013,7 @@
       </c>
       <c r="B338">
         <f t="shared" ca="1" si="5"/>
-        <v>553.70056025713268</v>
+        <v>557.25557715269667</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
@@ -23022,7 +23022,7 @@
       </c>
       <c r="B339">
         <f t="shared" ca="1" si="5"/>
-        <v>553.76206353927444</v>
+        <v>557.25690895452453</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -23031,7 +23031,7 @@
       </c>
       <c r="B340">
         <f t="shared" ca="1" si="5"/>
-        <v>553.83205749233741</v>
+        <v>557.3272790204461</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
@@ -23040,7 +23040,7 @@
       </c>
       <c r="B341">
         <f t="shared" ca="1" si="5"/>
-        <v>553.88295461195264</v>
+        <v>557.36484447187661</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
@@ -23049,7 +23049,7 @@
       </c>
       <c r="B342">
         <f t="shared" ca="1" si="5"/>
-        <v>553.94691905231048</v>
+        <v>557.42346620215676</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -23058,7 +23058,7 @@
       </c>
       <c r="B343">
         <f t="shared" ca="1" si="5"/>
-        <v>553.98465160898229</v>
+        <v>557.51624412015724</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
@@ -23067,7 +23067,7 @@
       </c>
       <c r="B344">
         <f t="shared" ca="1" si="5"/>
-        <v>553.99906594193897</v>
+        <v>557.56218315473382</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
@@ -23076,7 +23076,7 @@
       </c>
       <c r="B345">
         <f t="shared" ca="1" si="5"/>
-        <v>554.08055686271882</v>
+        <v>557.60908661813107</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -23085,7 +23085,7 @@
       </c>
       <c r="B346">
         <f t="shared" ca="1" si="5"/>
-        <v>554.15391208127789</v>
+        <v>557.61744248170351</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
@@ -23094,7 +23094,7 @@
       </c>
       <c r="B347">
         <f t="shared" ca="1" si="5"/>
-        <v>554.2146463915974</v>
+        <v>557.64359436649988</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
@@ -23103,7 +23103,7 @@
       </c>
       <c r="B348">
         <f t="shared" ca="1" si="5"/>
-        <v>554.22051377030004</v>
+        <v>557.69573155522676</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -23112,7 +23112,7 @@
       </c>
       <c r="B349">
         <f t="shared" ca="1" si="5"/>
-        <v>554.31482536587043</v>
+        <v>557.69643423774858</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
@@ -23121,7 +23121,7 @@
       </c>
       <c r="B350">
         <f t="shared" ca="1" si="5"/>
-        <v>554.38104697491667</v>
+        <v>557.79331182139742</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
@@ -23130,7 +23130,7 @@
       </c>
       <c r="B351">
         <f t="shared" ca="1" si="5"/>
-        <v>554.48077732368313</v>
+        <v>557.80251192121057</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -23139,7 +23139,7 @@
       </c>
       <c r="B352">
         <f t="shared" ca="1" si="5"/>
-        <v>554.54298569489868</v>
+        <v>557.9011926584011</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
@@ -23148,7 +23148,7 @@
       </c>
       <c r="B353">
         <f t="shared" ca="1" si="5"/>
-        <v>554.58342051052944</v>
+        <v>557.96955675968991</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
@@ -23157,7 +23157,7 @@
       </c>
       <c r="B354">
         <f t="shared" ca="1" si="5"/>
-        <v>554.68235461735401</v>
+        <v>558.01502064166107</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -23166,7 +23166,7 @@
       </c>
       <c r="B355">
         <f t="shared" ca="1" si="5"/>
-        <v>554.72721854432245</v>
+        <v>558.03418883511858</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
@@ -23175,7 +23175,7 @@
       </c>
       <c r="B356">
         <f t="shared" ca="1" si="5"/>
-        <v>554.76377785908267</v>
+        <v>558.12421172100244</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
@@ -23184,7 +23184,7 @@
       </c>
       <c r="B357">
         <f t="shared" ca="1" si="5"/>
-        <v>554.8574827233698</v>
+        <v>558.1824442861207</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -23193,7 +23193,7 @@
       </c>
       <c r="B358">
         <f t="shared" ca="1" si="5"/>
-        <v>554.94143030026191</v>
+        <v>558.2494533617363</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
@@ -23202,7 +23202,7 @@
       </c>
       <c r="B359">
         <f t="shared" ca="1" si="5"/>
-        <v>555.00696425216518</v>
+        <v>558.34360419363429</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
@@ -23211,7 +23211,7 @@
       </c>
       <c r="B360">
         <f t="shared" ca="1" si="5"/>
-        <v>555.02747168159578</v>
+        <v>558.41917670799444</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -23220,7 +23220,7 @@
       </c>
       <c r="B361">
         <f t="shared" ca="1" si="5"/>
-        <v>555.06978777861298</v>
+        <v>558.49474159541046</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
@@ -23229,7 +23229,7 @@
       </c>
       <c r="B362">
         <f t="shared" ca="1" si="5"/>
-        <v>555.09151984360972</v>
+        <v>558.57151634777301</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
@@ -23238,7 +23238,7 @@
       </c>
       <c r="B363">
         <f t="shared" ca="1" si="5"/>
-        <v>555.18396003301996</v>
+        <v>558.57340089328216</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -23247,7 +23247,7 @@
       </c>
       <c r="B364">
         <f t="shared" ca="1" si="5"/>
-        <v>555.18746433849128</v>
+        <v>558.63522892840285</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
@@ -23256,7 +23256,7 @@
       </c>
       <c r="B365">
         <f t="shared" ca="1" si="5"/>
-        <v>555.20344463653669</v>
+        <v>558.73045428434148</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
@@ -23265,7 +23265,7 @@
       </c>
       <c r="B366">
         <f t="shared" ca="1" si="5"/>
-        <v>555.20838021659972</v>
+        <v>558.75685625578694</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -23274,7 +23274,7 @@
       </c>
       <c r="B367">
         <f t="shared" ca="1" si="5"/>
-        <v>555.25772742796096</v>
+        <v>558.81098865700119</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
@@ -23283,7 +23283,7 @@
       </c>
       <c r="B368">
         <f t="shared" ca="1" si="5"/>
-        <v>555.31506948477295</v>
+        <v>558.8734161368684</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
@@ -23292,7 +23292,7 @@
       </c>
       <c r="B369">
         <f t="shared" ca="1" si="5"/>
-        <v>555.33666396353874</v>
+        <v>558.91515116748189</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -23301,7 +23301,7 @@
       </c>
       <c r="B370">
         <f t="shared" ca="1" si="5"/>
-        <v>555.43206520762794</v>
+        <v>558.94190823114354</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
@@ -23310,7 +23310,7 @@
       </c>
       <c r="B371">
         <f t="shared" ref="B371:B402" ca="1" si="6">B370+0.1*RAND()</f>
-        <v>555.51707018998434</v>
+        <v>559.01106413416949</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -23319,7 +23319,7 @@
       </c>
       <c r="B372">
         <f t="shared" ca="1" si="6"/>
-        <v>555.55053331555143</v>
+        <v>559.03533228188678</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -23328,7 +23328,7 @@
       </c>
       <c r="B373">
         <f t="shared" ca="1" si="6"/>
-        <v>555.59470319469244</v>
+        <v>559.13246831799279</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
@@ -23337,7 +23337,7 @@
       </c>
       <c r="B374">
         <f t="shared" ca="1" si="6"/>
-        <v>555.63064971069537</v>
+        <v>559.18639107658089</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -23346,7 +23346,7 @@
       </c>
       <c r="B375">
         <f t="shared" ca="1" si="6"/>
-        <v>555.63318674864149</v>
+        <v>559.25831133447741</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -23355,7 +23355,7 @@
       </c>
       <c r="B376">
         <f t="shared" ca="1" si="6"/>
-        <v>555.67766654548245</v>
+        <v>559.34841842364392</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
@@ -23364,7 +23364,7 @@
       </c>
       <c r="B377">
         <f t="shared" ca="1" si="6"/>
-        <v>555.70167951458461</v>
+        <v>559.42128859514833</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
@@ -23373,7 +23373,7 @@
       </c>
       <c r="B378">
         <f t="shared" ca="1" si="6"/>
-        <v>555.73732947342069</v>
+        <v>559.49631013735723</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -23382,7 +23382,7 @@
       </c>
       <c r="B379">
         <f t="shared" ca="1" si="6"/>
-        <v>555.81451193576424</v>
+        <v>559.53808565005716</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
@@ -23391,7 +23391,7 @@
       </c>
       <c r="B380">
         <f t="shared" ca="1" si="6"/>
-        <v>555.87916497856008</v>
+        <v>559.61728002314896</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
@@ -23400,7 +23400,7 @@
       </c>
       <c r="B381">
         <f t="shared" ca="1" si="6"/>
-        <v>555.9228650509308</v>
+        <v>559.69344852888071</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -23409,7 +23409,7 @@
       </c>
       <c r="B382">
         <f t="shared" ca="1" si="6"/>
-        <v>555.95813404345813</v>
+        <v>559.69530941700759</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
@@ -23418,7 +23418,7 @@
       </c>
       <c r="B383">
         <f t="shared" ca="1" si="6"/>
-        <v>556.04062711813765</v>
+        <v>559.75221312927647</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
@@ -23427,7 +23427,7 @@
       </c>
       <c r="B384">
         <f t="shared" ca="1" si="6"/>
-        <v>556.09530573906397</v>
+        <v>559.81632452809743</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -23436,7 +23436,7 @@
       </c>
       <c r="B385">
         <f t="shared" ca="1" si="6"/>
-        <v>556.1515438445881</v>
+        <v>559.84640871671627</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
@@ -23445,7 +23445,7 @@
       </c>
       <c r="B386">
         <f t="shared" ca="1" si="6"/>
-        <v>556.24493074015231</v>
+        <v>559.91684542146118</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
@@ -23454,7 +23454,7 @@
       </c>
       <c r="B387">
         <f t="shared" ca="1" si="6"/>
-        <v>556.31270267935611</v>
+        <v>559.91976319751723</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -23463,7 +23463,7 @@
       </c>
       <c r="B388">
         <f t="shared" ca="1" si="6"/>
-        <v>556.3994491546415</v>
+        <v>559.93497995676546</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
@@ -23472,7 +23472,7 @@
       </c>
       <c r="B389">
         <f t="shared" ca="1" si="6"/>
-        <v>556.40751516088574</v>
+        <v>559.95830463998516</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
@@ -23481,7 +23481,7 @@
       </c>
       <c r="B390">
         <f t="shared" ca="1" si="6"/>
-        <v>556.48650422140997</v>
+        <v>560.01214775829226</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -23490,7 +23490,7 @@
       </c>
       <c r="B391">
         <f t="shared" ca="1" si="6"/>
-        <v>556.53484592641803</v>
+        <v>560.10411319451975</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
@@ -23499,7 +23499,7 @@
       </c>
       <c r="B392">
         <f t="shared" ca="1" si="6"/>
-        <v>556.54657422622449</v>
+        <v>560.20051319756624</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
@@ -23508,7 +23508,7 @@
       </c>
       <c r="B393">
         <f t="shared" ca="1" si="6"/>
-        <v>556.60352327914381</v>
+        <v>560.25686491301246</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -23517,7 +23517,7 @@
       </c>
       <c r="B394">
         <f t="shared" ca="1" si="6"/>
-        <v>556.65220921529544</v>
+        <v>560.32708192318728</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
@@ -23526,7 +23526,7 @@
       </c>
       <c r="B395">
         <f t="shared" ca="1" si="6"/>
-        <v>556.71808311932205</v>
+        <v>560.3931668531892</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
@@ -23535,7 +23535,7 @@
       </c>
       <c r="B396">
         <f t="shared" ca="1" si="6"/>
-        <v>556.79070233791163</v>
+        <v>560.42683880283244</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -23544,7 +23544,7 @@
       </c>
       <c r="B397">
         <f t="shared" ca="1" si="6"/>
-        <v>556.85208146472951</v>
+        <v>560.51706798996099</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
@@ -23553,7 +23553,7 @@
       </c>
       <c r="B398">
         <f t="shared" ca="1" si="6"/>
-        <v>556.87910807846356</v>
+        <v>560.57354569556844</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
@@ -23562,7 +23562,7 @@
       </c>
       <c r="B399">
         <f t="shared" ca="1" si="6"/>
-        <v>556.88121950308607</v>
+        <v>560.63238316636739</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -23571,7 +23571,7 @@
       </c>
       <c r="B400">
         <f t="shared" ca="1" si="6"/>
-        <v>556.946909469753</v>
+        <v>560.67067870935637</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
@@ -23580,7 +23580,7 @@
       </c>
       <c r="B401">
         <f t="shared" ca="1" si="6"/>
-        <v>557.00043422138492</v>
+        <v>560.75952940342722</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
@@ -23589,7 +23589,7 @@
       </c>
       <c r="B402">
         <f t="shared" ca="1" si="6"/>
-        <v>557.02206782482301</v>
+        <v>560.80875836382813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>